<commit_message>
DRC errors removed Cutouts improved Logo test added
</commit_message>
<xml_diff>
--- a/Karman Delta Arm/Rocket arming system.xlsx
+++ b/Karman Delta Arm/Rocket arming system.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adria\Documents\GitHub\AltiumGithub\Karman Delta Arm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06FF8978-0DAF-4F0A-99E5-B5A1731636B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83159B67-4154-458D-B4A4-41D4EA42FB8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2220" windowWidth="21600" windowHeight="12645" tabRatio="745" activeTab="4" xr2:uid="{C397F53C-48EF-47A2-AFE9-4806826F5736}"/>
+    <workbookView xWindow="37965" yWindow="2010" windowWidth="21600" windowHeight="12645" tabRatio="745" activeTab="4" xr2:uid="{C397F53C-48EF-47A2-AFE9-4806826F5736}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="397">
   <si>
     <t>Failure Mode</t>
   </si>
@@ -1659,23 +1659,113 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1684,96 +1774,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3906,8 +3906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90E11162-B732-4DE9-8322-FD8094AB6283}">
   <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -3994,6 +3994,9 @@
       <c r="A11" s="1" t="s">
         <v>47</v>
       </c>
+      <c r="B11" s="6" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="12" spans="1:3" ht="14.25">
       <c r="A12" s="1" t="s">
@@ -4039,6 +4042,9 @@
       <c r="A18" s="1" t="s">
         <v>257</v>
       </c>
+      <c r="B18" s="6" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="1" t="s">
@@ -4117,6 +4123,9 @@
       <c r="A30" s="1" t="s">
         <v>377</v>
       </c>
+      <c r="B30" s="6" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="1" t="s">
@@ -4135,6 +4144,9 @@
       <c r="A33" s="1" t="s">
         <v>380</v>
       </c>
+      <c r="B33" s="6" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="1" t="s">
@@ -4153,11 +4165,17 @@
       <c r="A36" s="1" t="s">
         <v>383</v>
       </c>
+      <c r="B36" s="6" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="1" t="s">
         <v>384</v>
       </c>
+      <c r="B37" s="6" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="1" t="s">
@@ -4196,6 +4214,9 @@
       <c r="A44" s="1" t="s">
         <v>391</v>
       </c>
+      <c r="B44" s="6" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="1" t="s">
@@ -4205,6 +4226,9 @@
     <row r="46" spans="1:2" ht="30">
       <c r="A46" s="1" t="s">
         <v>393</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -4401,31 +4425,31 @@
   <sheetData>
     <row r="2" spans="2:16" ht="15" thickBot="1"/>
     <row r="3" spans="2:16" ht="15" thickBot="1">
-      <c r="B3" s="76" t="s">
+      <c r="B3" s="48" t="s">
         <v>79</v>
       </c>
-      <c r="C3" s="77"/>
-      <c r="D3" s="77"/>
-      <c r="E3" s="77"/>
-      <c r="F3" s="77"/>
-      <c r="G3" s="77"/>
-      <c r="H3" s="78"/>
-      <c r="I3" s="83" t="s">
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="54" t="s">
         <v>234</v>
       </c>
-      <c r="J3" s="79" t="s">
+      <c r="J3" s="64" t="s">
         <v>232</v>
       </c>
-      <c r="K3" s="79" t="s">
+      <c r="K3" s="64" t="s">
         <v>233</v>
       </c>
-      <c r="L3" s="81" t="s">
+      <c r="L3" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="M3" s="76" t="s">
+      <c r="M3" s="48" t="s">
         <v>80</v>
       </c>
-      <c r="N3" s="78"/>
+      <c r="N3" s="49"/>
     </row>
     <row r="4" spans="2:16" ht="96.75" customHeight="1" thickBot="1">
       <c r="B4" s="27" t="s">
@@ -4449,10 +4473,10 @@
       <c r="H4" s="28" t="s">
         <v>231</v>
       </c>
-      <c r="I4" s="84"/>
-      <c r="J4" s="80"/>
-      <c r="K4" s="80"/>
-      <c r="L4" s="82"/>
+      <c r="I4" s="55"/>
+      <c r="J4" s="65"/>
+      <c r="K4" s="65"/>
+      <c r="L4" s="47"/>
       <c r="M4" s="11" t="s">
         <v>81</v>
       </c>
@@ -4464,43 +4488,43 @@
       </c>
     </row>
     <row r="5" spans="2:16" ht="15" thickTop="1">
-      <c r="B5" s="62">
+      <c r="B5" s="50">
         <v>2</v>
       </c>
-      <c r="C5" s="62">
+      <c r="C5" s="50">
         <v>1</v>
       </c>
-      <c r="D5" s="62">
+      <c r="D5" s="50">
         <v>2</v>
       </c>
-      <c r="E5" s="62">
+      <c r="E5" s="50">
         <v>2</v>
       </c>
-      <c r="F5" s="63">
+      <c r="F5" s="52">
         <v>2</v>
       </c>
-      <c r="G5" s="62">
+      <c r="G5" s="50">
         <v>2</v>
       </c>
-      <c r="H5" s="71" t="s">
+      <c r="H5" s="58" t="s">
         <v>83</v>
       </c>
       <c r="I5" s="38" t="s">
         <v>84</v>
       </c>
-      <c r="J5" s="62" t="s">
+      <c r="J5" s="50" t="s">
         <v>86</v>
       </c>
-      <c r="K5" s="62" t="s">
+      <c r="K5" s="50" t="s">
         <v>87</v>
       </c>
-      <c r="L5" s="61" t="s">
-        <v>88</v>
-      </c>
-      <c r="M5" s="61" t="s">
-        <v>88</v>
-      </c>
-      <c r="N5" s="61" t="s">
+      <c r="L5" s="56" t="s">
+        <v>88</v>
+      </c>
+      <c r="M5" s="56" t="s">
+        <v>88</v>
+      </c>
+      <c r="N5" s="56" t="s">
         <v>85</v>
       </c>
       <c r="P5" t="s">
@@ -4512,56 +4536,56 @@
       <c r="C6" s="51"/>
       <c r="D6" s="51"/>
       <c r="E6" s="51"/>
-      <c r="F6" s="60"/>
+      <c r="F6" s="53"/>
       <c r="G6" s="51"/>
-      <c r="H6" s="57"/>
+      <c r="H6" s="59"/>
       <c r="I6" s="15" t="s">
         <v>85</v>
       </c>
       <c r="J6" s="51"/>
       <c r="K6" s="51"/>
-      <c r="L6" s="48"/>
-      <c r="M6" s="48"/>
-      <c r="N6" s="48"/>
+      <c r="L6" s="57"/>
+      <c r="M6" s="57"/>
+      <c r="N6" s="57"/>
     </row>
     <row r="7" spans="2:16">
-      <c r="B7" s="49">
+      <c r="B7" s="60">
         <v>3</v>
       </c>
-      <c r="C7" s="49">
+      <c r="C7" s="60">
         <v>2</v>
       </c>
-      <c r="D7" s="49">
+      <c r="D7" s="60">
         <v>3</v>
       </c>
-      <c r="E7" s="49">
+      <c r="E7" s="60">
         <v>3</v>
       </c>
-      <c r="F7" s="58">
+      <c r="F7" s="61">
         <v>3</v>
       </c>
-      <c r="G7" s="49">
+      <c r="G7" s="60">
         <v>3</v>
       </c>
-      <c r="H7" s="55" t="s">
+      <c r="H7" s="62" t="s">
         <v>89</v>
       </c>
       <c r="I7" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="J7" s="49" t="s">
+      <c r="J7" s="60" t="s">
         <v>86</v>
       </c>
-      <c r="K7" s="49" t="s">
+      <c r="K7" s="60" t="s">
         <v>92</v>
       </c>
-      <c r="L7" s="46" t="s">
-        <v>88</v>
-      </c>
-      <c r="M7" s="46" t="s">
-        <v>88</v>
-      </c>
-      <c r="N7" s="46" t="s">
+      <c r="L7" s="68" t="s">
+        <v>88</v>
+      </c>
+      <c r="M7" s="68" t="s">
+        <v>88</v>
+      </c>
+      <c r="N7" s="68" t="s">
         <v>91</v>
       </c>
       <c r="P7" t="s">
@@ -4573,17 +4597,17 @@
       <c r="C8" s="51"/>
       <c r="D8" s="51"/>
       <c r="E8" s="51"/>
-      <c r="F8" s="60"/>
+      <c r="F8" s="53"/>
       <c r="G8" s="51"/>
-      <c r="H8" s="57"/>
+      <c r="H8" s="59"/>
       <c r="I8" s="16" t="s">
         <v>91</v>
       </c>
       <c r="J8" s="51"/>
       <c r="K8" s="51"/>
-      <c r="L8" s="48"/>
-      <c r="M8" s="48"/>
-      <c r="N8" s="48"/>
+      <c r="L8" s="57"/>
+      <c r="M8" s="57"/>
+      <c r="N8" s="57"/>
     </row>
     <row r="9" spans="2:16" ht="15" thickBot="1">
       <c r="B9" s="17">
@@ -4668,37 +4692,37 @@
       </c>
     </row>
     <row r="11" spans="2:16" ht="24">
-      <c r="B11" s="49">
+      <c r="B11" s="60">
         <v>5</v>
       </c>
-      <c r="C11" s="49">
+      <c r="C11" s="60">
         <v>5</v>
       </c>
-      <c r="D11" s="49">
+      <c r="D11" s="60">
         <v>6</v>
       </c>
-      <c r="E11" s="49">
+      <c r="E11" s="60">
         <v>6</v>
       </c>
-      <c r="F11" s="58">
+      <c r="F11" s="61">
         <v>6</v>
       </c>
-      <c r="G11" s="49">
+      <c r="G11" s="60">
         <v>6</v>
       </c>
-      <c r="H11" s="55" t="s">
+      <c r="H11" s="62" t="s">
         <v>100</v>
       </c>
-      <c r="I11" s="73" t="s">
+      <c r="I11" s="71" t="s">
         <v>101</v>
       </c>
-      <c r="J11" s="49" t="s">
+      <c r="J11" s="60" t="s">
         <v>86</v>
       </c>
-      <c r="K11" s="55" t="s">
+      <c r="K11" s="62" t="s">
         <v>102</v>
       </c>
-      <c r="L11" s="46" t="s">
+      <c r="L11" s="68" t="s">
         <v>88</v>
       </c>
       <c r="M11" s="29" t="s">
@@ -4712,17 +4736,17 @@
       </c>
     </row>
     <row r="12" spans="2:16" ht="24">
-      <c r="B12" s="50"/>
-      <c r="C12" s="50"/>
-      <c r="D12" s="50"/>
-      <c r="E12" s="50"/>
-      <c r="F12" s="59"/>
-      <c r="G12" s="50"/>
-      <c r="H12" s="56"/>
-      <c r="I12" s="74"/>
-      <c r="J12" s="50"/>
-      <c r="K12" s="56"/>
-      <c r="L12" s="47"/>
+      <c r="B12" s="66"/>
+      <c r="C12" s="66"/>
+      <c r="D12" s="66"/>
+      <c r="E12" s="66"/>
+      <c r="F12" s="67"/>
+      <c r="G12" s="66"/>
+      <c r="H12" s="69"/>
+      <c r="I12" s="72"/>
+      <c r="J12" s="66"/>
+      <c r="K12" s="69"/>
+      <c r="L12" s="70"/>
       <c r="M12" s="14" t="s">
         <v>104</v>
       </c>
@@ -4731,17 +4755,17 @@
       </c>
     </row>
     <row r="13" spans="2:16" ht="24">
-      <c r="B13" s="50"/>
-      <c r="C13" s="50"/>
-      <c r="D13" s="50"/>
-      <c r="E13" s="50"/>
-      <c r="F13" s="59"/>
-      <c r="G13" s="50"/>
-      <c r="H13" s="56"/>
-      <c r="I13" s="74"/>
-      <c r="J13" s="50"/>
-      <c r="K13" s="56"/>
-      <c r="L13" s="47"/>
+      <c r="B13" s="66"/>
+      <c r="C13" s="66"/>
+      <c r="D13" s="66"/>
+      <c r="E13" s="66"/>
+      <c r="F13" s="67"/>
+      <c r="G13" s="66"/>
+      <c r="H13" s="69"/>
+      <c r="I13" s="72"/>
+      <c r="J13" s="66"/>
+      <c r="K13" s="69"/>
+      <c r="L13" s="70"/>
       <c r="M13" s="14" t="s">
         <v>105</v>
       </c>
@@ -4750,17 +4774,17 @@
       </c>
     </row>
     <row r="14" spans="2:16" ht="36">
-      <c r="B14" s="50"/>
-      <c r="C14" s="50"/>
-      <c r="D14" s="50"/>
-      <c r="E14" s="50"/>
-      <c r="F14" s="59"/>
-      <c r="G14" s="50"/>
-      <c r="H14" s="56"/>
-      <c r="I14" s="74"/>
-      <c r="J14" s="50"/>
-      <c r="K14" s="56"/>
-      <c r="L14" s="47"/>
+      <c r="B14" s="66"/>
+      <c r="C14" s="66"/>
+      <c r="D14" s="66"/>
+      <c r="E14" s="66"/>
+      <c r="F14" s="67"/>
+      <c r="G14" s="66"/>
+      <c r="H14" s="69"/>
+      <c r="I14" s="72"/>
+      <c r="J14" s="66"/>
+      <c r="K14" s="69"/>
+      <c r="L14" s="70"/>
       <c r="M14" s="14" t="s">
         <v>106</v>
       </c>
@@ -4769,17 +4793,17 @@
       </c>
     </row>
     <row r="15" spans="2:16" ht="24">
-      <c r="B15" s="50"/>
-      <c r="C15" s="50"/>
-      <c r="D15" s="50"/>
-      <c r="E15" s="50"/>
-      <c r="F15" s="59"/>
-      <c r="G15" s="50"/>
-      <c r="H15" s="56"/>
-      <c r="I15" s="74"/>
-      <c r="J15" s="50"/>
-      <c r="K15" s="56"/>
-      <c r="L15" s="47"/>
+      <c r="B15" s="66"/>
+      <c r="C15" s="66"/>
+      <c r="D15" s="66"/>
+      <c r="E15" s="66"/>
+      <c r="F15" s="67"/>
+      <c r="G15" s="66"/>
+      <c r="H15" s="69"/>
+      <c r="I15" s="72"/>
+      <c r="J15" s="66"/>
+      <c r="K15" s="69"/>
+      <c r="L15" s="70"/>
       <c r="M15" s="29" t="s">
         <v>107</v>
       </c>
@@ -4790,50 +4814,50 @@
       <c r="C16" s="51"/>
       <c r="D16" s="51"/>
       <c r="E16" s="51"/>
-      <c r="F16" s="60"/>
+      <c r="F16" s="53"/>
       <c r="G16" s="51"/>
-      <c r="H16" s="57"/>
-      <c r="I16" s="75"/>
+      <c r="H16" s="59"/>
+      <c r="I16" s="73"/>
       <c r="J16" s="51"/>
-      <c r="K16" s="57"/>
-      <c r="L16" s="48"/>
+      <c r="K16" s="59"/>
+      <c r="L16" s="57"/>
       <c r="M16" s="21" t="s">
         <v>108</v>
       </c>
       <c r="N16" s="18"/>
     </row>
     <row r="17" spans="2:16" ht="24">
-      <c r="B17" s="49">
+      <c r="B17" s="60">
         <v>6</v>
       </c>
-      <c r="C17" s="49">
+      <c r="C17" s="60">
         <v>6</v>
       </c>
-      <c r="D17" s="49">
+      <c r="D17" s="60">
         <v>7</v>
       </c>
-      <c r="E17" s="49">
+      <c r="E17" s="60">
         <v>7</v>
       </c>
-      <c r="F17" s="58">
+      <c r="F17" s="61">
         <v>7</v>
       </c>
-      <c r="G17" s="49">
+      <c r="G17" s="60">
         <v>7</v>
       </c>
-      <c r="H17" s="55" t="s">
+      <c r="H17" s="62" t="s">
         <v>113</v>
       </c>
-      <c r="I17" s="46" t="s">
+      <c r="I17" s="68" t="s">
         <v>114</v>
       </c>
-      <c r="J17" s="49" t="s">
+      <c r="J17" s="60" t="s">
         <v>86</v>
       </c>
-      <c r="K17" s="49" t="s">
+      <c r="K17" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="L17" s="46" t="s">
+      <c r="L17" s="68" t="s">
         <v>88</v>
       </c>
       <c r="M17" s="23" t="s">
@@ -4844,17 +4868,17 @@
       </c>
     </row>
     <row r="18" spans="2:16" ht="24">
-      <c r="B18" s="50"/>
-      <c r="C18" s="50"/>
-      <c r="D18" s="50"/>
-      <c r="E18" s="50"/>
-      <c r="F18" s="59"/>
-      <c r="G18" s="50"/>
-      <c r="H18" s="56"/>
-      <c r="I18" s="47"/>
-      <c r="J18" s="50"/>
-      <c r="K18" s="50"/>
-      <c r="L18" s="47"/>
+      <c r="B18" s="66"/>
+      <c r="C18" s="66"/>
+      <c r="D18" s="66"/>
+      <c r="E18" s="66"/>
+      <c r="F18" s="67"/>
+      <c r="G18" s="66"/>
+      <c r="H18" s="69"/>
+      <c r="I18" s="70"/>
+      <c r="J18" s="66"/>
+      <c r="K18" s="66"/>
+      <c r="L18" s="70"/>
       <c r="M18" s="23" t="s">
         <v>116</v>
       </c>
@@ -4863,68 +4887,68 @@
       </c>
     </row>
     <row r="19" spans="2:16">
-      <c r="B19" s="50"/>
-      <c r="C19" s="50"/>
-      <c r="D19" s="50"/>
-      <c r="E19" s="50"/>
-      <c r="F19" s="59"/>
-      <c r="G19" s="50"/>
-      <c r="H19" s="56"/>
-      <c r="I19" s="47"/>
-      <c r="J19" s="50"/>
-      <c r="K19" s="50"/>
-      <c r="L19" s="47"/>
+      <c r="B19" s="66"/>
+      <c r="C19" s="66"/>
+      <c r="D19" s="66"/>
+      <c r="E19" s="66"/>
+      <c r="F19" s="67"/>
+      <c r="G19" s="66"/>
+      <c r="H19" s="69"/>
+      <c r="I19" s="70"/>
+      <c r="J19" s="66"/>
+      <c r="K19" s="66"/>
+      <c r="L19" s="70"/>
       <c r="M19" s="14" t="s">
         <v>117</v>
       </c>
       <c r="N19" s="26"/>
     </row>
     <row r="20" spans="2:16" ht="24">
-      <c r="B20" s="50"/>
-      <c r="C20" s="50"/>
-      <c r="D20" s="50"/>
-      <c r="E20" s="50"/>
-      <c r="F20" s="59"/>
-      <c r="G20" s="50"/>
-      <c r="H20" s="56"/>
-      <c r="I20" s="47"/>
-      <c r="J20" s="50"/>
-      <c r="K20" s="50"/>
-      <c r="L20" s="47"/>
+      <c r="B20" s="66"/>
+      <c r="C20" s="66"/>
+      <c r="D20" s="66"/>
+      <c r="E20" s="66"/>
+      <c r="F20" s="67"/>
+      <c r="G20" s="66"/>
+      <c r="H20" s="69"/>
+      <c r="I20" s="70"/>
+      <c r="J20" s="66"/>
+      <c r="K20" s="66"/>
+      <c r="L20" s="70"/>
       <c r="M20" s="23" t="s">
         <v>118</v>
       </c>
       <c r="N20" s="26"/>
     </row>
     <row r="21" spans="2:16" ht="24">
-      <c r="B21" s="50"/>
-      <c r="C21" s="50"/>
-      <c r="D21" s="50"/>
-      <c r="E21" s="50"/>
-      <c r="F21" s="59"/>
-      <c r="G21" s="50"/>
-      <c r="H21" s="56"/>
-      <c r="I21" s="47"/>
-      <c r="J21" s="50"/>
-      <c r="K21" s="50"/>
-      <c r="L21" s="47"/>
+      <c r="B21" s="66"/>
+      <c r="C21" s="66"/>
+      <c r="D21" s="66"/>
+      <c r="E21" s="66"/>
+      <c r="F21" s="67"/>
+      <c r="G21" s="66"/>
+      <c r="H21" s="69"/>
+      <c r="I21" s="70"/>
+      <c r="J21" s="66"/>
+      <c r="K21" s="66"/>
+      <c r="L21" s="70"/>
       <c r="M21" s="13" t="s">
         <v>119</v>
       </c>
       <c r="N21" s="26"/>
     </row>
     <row r="22" spans="2:16" ht="24">
-      <c r="B22" s="50"/>
-      <c r="C22" s="50"/>
-      <c r="D22" s="50"/>
-      <c r="E22" s="50"/>
-      <c r="F22" s="59"/>
-      <c r="G22" s="50"/>
-      <c r="H22" s="56"/>
-      <c r="I22" s="47"/>
-      <c r="J22" s="50"/>
-      <c r="K22" s="50"/>
-      <c r="L22" s="47"/>
+      <c r="B22" s="66"/>
+      <c r="C22" s="66"/>
+      <c r="D22" s="66"/>
+      <c r="E22" s="66"/>
+      <c r="F22" s="67"/>
+      <c r="G22" s="66"/>
+      <c r="H22" s="69"/>
+      <c r="I22" s="70"/>
+      <c r="J22" s="66"/>
+      <c r="K22" s="66"/>
+      <c r="L22" s="70"/>
       <c r="M22" s="14" t="s">
         <v>120</v>
       </c>
@@ -4935,50 +4959,50 @@
       <c r="C23" s="51"/>
       <c r="D23" s="51"/>
       <c r="E23" s="51"/>
-      <c r="F23" s="60"/>
+      <c r="F23" s="53"/>
       <c r="G23" s="51"/>
-      <c r="H23" s="57"/>
-      <c r="I23" s="48"/>
+      <c r="H23" s="59"/>
+      <c r="I23" s="57"/>
       <c r="J23" s="51"/>
       <c r="K23" s="51"/>
-      <c r="L23" s="48"/>
+      <c r="L23" s="57"/>
       <c r="M23" s="40" t="s">
         <v>121</v>
       </c>
       <c r="N23" s="24"/>
     </row>
     <row r="24" spans="2:16" ht="36">
-      <c r="B24" s="46" t="s">
-        <v>88</v>
-      </c>
-      <c r="C24" s="46" t="s">
-        <v>88</v>
-      </c>
-      <c r="D24" s="49">
+      <c r="B24" s="68" t="s">
+        <v>88</v>
+      </c>
+      <c r="C24" s="68" t="s">
+        <v>88</v>
+      </c>
+      <c r="D24" s="60">
         <v>8</v>
       </c>
-      <c r="E24" s="49">
+      <c r="E24" s="60">
         <v>8</v>
       </c>
-      <c r="F24" s="58">
+      <c r="F24" s="61">
         <v>8</v>
       </c>
-      <c r="G24" s="49">
+      <c r="G24" s="60">
         <v>8</v>
       </c>
-      <c r="H24" s="55" t="s">
+      <c r="H24" s="62" t="s">
         <v>122</v>
       </c>
-      <c r="I24" s="46" t="s">
+      <c r="I24" s="68" t="s">
         <v>123</v>
       </c>
-      <c r="J24" s="49" t="s">
+      <c r="J24" s="60" t="s">
         <v>86</v>
       </c>
-      <c r="K24" s="55" t="s">
+      <c r="K24" s="62" t="s">
         <v>102</v>
       </c>
-      <c r="L24" s="46" t="s">
+      <c r="L24" s="68" t="s">
         <v>88</v>
       </c>
       <c r="M24" s="14" t="s">
@@ -4989,17 +5013,17 @@
       </c>
     </row>
     <row r="25" spans="2:16" ht="24">
-      <c r="B25" s="47"/>
-      <c r="C25" s="47"/>
-      <c r="D25" s="50"/>
-      <c r="E25" s="50"/>
-      <c r="F25" s="59"/>
-      <c r="G25" s="50"/>
-      <c r="H25" s="56"/>
-      <c r="I25" s="47"/>
-      <c r="J25" s="50"/>
-      <c r="K25" s="56"/>
-      <c r="L25" s="47"/>
+      <c r="B25" s="70"/>
+      <c r="C25" s="70"/>
+      <c r="D25" s="66"/>
+      <c r="E25" s="66"/>
+      <c r="F25" s="67"/>
+      <c r="G25" s="66"/>
+      <c r="H25" s="69"/>
+      <c r="I25" s="70"/>
+      <c r="J25" s="66"/>
+      <c r="K25" s="69"/>
+      <c r="L25" s="70"/>
       <c r="M25" s="29" t="s">
         <v>125</v>
       </c>
@@ -5011,17 +5035,17 @@
       </c>
     </row>
     <row r="26" spans="2:16" ht="24">
-      <c r="B26" s="47"/>
-      <c r="C26" s="47"/>
-      <c r="D26" s="50"/>
-      <c r="E26" s="50"/>
-      <c r="F26" s="59"/>
-      <c r="G26" s="50"/>
-      <c r="H26" s="56"/>
-      <c r="I26" s="47"/>
-      <c r="J26" s="50"/>
-      <c r="K26" s="56"/>
-      <c r="L26" s="47"/>
+      <c r="B26" s="70"/>
+      <c r="C26" s="70"/>
+      <c r="D26" s="66"/>
+      <c r="E26" s="66"/>
+      <c r="F26" s="67"/>
+      <c r="G26" s="66"/>
+      <c r="H26" s="69"/>
+      <c r="I26" s="70"/>
+      <c r="J26" s="66"/>
+      <c r="K26" s="69"/>
+      <c r="L26" s="70"/>
       <c r="M26" s="14" t="s">
         <v>126</v>
       </c>
@@ -5030,17 +5054,17 @@
       </c>
     </row>
     <row r="27" spans="2:16" ht="24.75" thickBot="1">
-      <c r="B27" s="48"/>
-      <c r="C27" s="48"/>
+      <c r="B27" s="57"/>
+      <c r="C27" s="57"/>
       <c r="D27" s="51"/>
       <c r="E27" s="51"/>
-      <c r="F27" s="60"/>
+      <c r="F27" s="53"/>
       <c r="G27" s="51"/>
-      <c r="H27" s="57"/>
-      <c r="I27" s="48"/>
+      <c r="H27" s="59"/>
+      <c r="I27" s="57"/>
       <c r="J27" s="51"/>
-      <c r="K27" s="57"/>
-      <c r="L27" s="48"/>
+      <c r="K27" s="59"/>
+      <c r="L27" s="57"/>
       <c r="M27" s="19" t="s">
         <v>127</v>
       </c>
@@ -5049,37 +5073,37 @@
       </c>
     </row>
     <row r="28" spans="2:16" ht="24">
-      <c r="B28" s="46" t="s">
-        <v>88</v>
-      </c>
-      <c r="C28" s="46" t="s">
-        <v>88</v>
-      </c>
-      <c r="D28" s="49">
+      <c r="B28" s="68" t="s">
+        <v>88</v>
+      </c>
+      <c r="C28" s="68" t="s">
+        <v>88</v>
+      </c>
+      <c r="D28" s="60">
         <v>9</v>
       </c>
-      <c r="E28" s="49">
+      <c r="E28" s="60">
         <v>9</v>
       </c>
-      <c r="F28" s="58">
+      <c r="F28" s="61">
         <v>9</v>
       </c>
-      <c r="G28" s="49">
+      <c r="G28" s="60">
         <v>9</v>
       </c>
-      <c r="H28" s="55" t="s">
+      <c r="H28" s="62" t="s">
         <v>132</v>
       </c>
-      <c r="I28" s="46" t="s">
+      <c r="I28" s="68" t="s">
         <v>133</v>
       </c>
-      <c r="J28" s="49" t="s">
+      <c r="J28" s="60" t="s">
         <v>86</v>
       </c>
-      <c r="K28" s="49" t="s">
+      <c r="K28" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="L28" s="46" t="s">
+      <c r="L28" s="68" t="s">
         <v>88</v>
       </c>
       <c r="M28" s="14" t="s">
@@ -5090,17 +5114,17 @@
       </c>
     </row>
     <row r="29" spans="2:16">
-      <c r="B29" s="47"/>
-      <c r="C29" s="47"/>
-      <c r="D29" s="50"/>
-      <c r="E29" s="50"/>
-      <c r="F29" s="59"/>
-      <c r="G29" s="50"/>
-      <c r="H29" s="56"/>
-      <c r="I29" s="47"/>
-      <c r="J29" s="50"/>
-      <c r="K29" s="50"/>
-      <c r="L29" s="47"/>
+      <c r="B29" s="70"/>
+      <c r="C29" s="70"/>
+      <c r="D29" s="66"/>
+      <c r="E29" s="66"/>
+      <c r="F29" s="67"/>
+      <c r="G29" s="66"/>
+      <c r="H29" s="69"/>
+      <c r="I29" s="70"/>
+      <c r="J29" s="66"/>
+      <c r="K29" s="66"/>
+      <c r="L29" s="70"/>
       <c r="M29" s="14" t="s">
         <v>135</v>
       </c>
@@ -5109,71 +5133,71 @@
       </c>
     </row>
     <row r="30" spans="2:16" ht="24">
-      <c r="B30" s="47"/>
-      <c r="C30" s="47"/>
-      <c r="D30" s="50"/>
-      <c r="E30" s="50"/>
-      <c r="F30" s="59"/>
-      <c r="G30" s="50"/>
-      <c r="H30" s="56"/>
-      <c r="I30" s="47"/>
-      <c r="J30" s="50"/>
-      <c r="K30" s="50"/>
-      <c r="L30" s="47"/>
+      <c r="B30" s="70"/>
+      <c r="C30" s="70"/>
+      <c r="D30" s="66"/>
+      <c r="E30" s="66"/>
+      <c r="F30" s="67"/>
+      <c r="G30" s="66"/>
+      <c r="H30" s="69"/>
+      <c r="I30" s="70"/>
+      <c r="J30" s="66"/>
+      <c r="K30" s="66"/>
+      <c r="L30" s="70"/>
       <c r="M30" s="29" t="s">
         <v>103</v>
       </c>
       <c r="N30" s="26"/>
     </row>
     <row r="31" spans="2:16" ht="24.75" thickBot="1">
-      <c r="B31" s="48"/>
-      <c r="C31" s="48"/>
+      <c r="B31" s="57"/>
+      <c r="C31" s="57"/>
       <c r="D31" s="51"/>
       <c r="E31" s="51"/>
-      <c r="F31" s="60"/>
+      <c r="F31" s="53"/>
       <c r="G31" s="51"/>
-      <c r="H31" s="57"/>
-      <c r="I31" s="48"/>
+      <c r="H31" s="59"/>
+      <c r="I31" s="57"/>
       <c r="J31" s="51"/>
       <c r="K31" s="51"/>
-      <c r="L31" s="48"/>
+      <c r="L31" s="57"/>
       <c r="M31" s="40" t="s">
         <v>136</v>
       </c>
       <c r="N31" s="24"/>
     </row>
     <row r="32" spans="2:16" ht="24">
-      <c r="B32" s="49">
+      <c r="B32" s="60">
         <v>7</v>
       </c>
-      <c r="C32" s="49">
+      <c r="C32" s="60">
         <v>7</v>
       </c>
-      <c r="D32" s="49">
+      <c r="D32" s="60">
         <v>10</v>
       </c>
-      <c r="E32" s="49">
+      <c r="E32" s="60">
         <v>10</v>
       </c>
-      <c r="F32" s="58">
+      <c r="F32" s="61">
         <v>10</v>
       </c>
-      <c r="G32" s="49">
+      <c r="G32" s="60">
         <v>10</v>
       </c>
-      <c r="H32" s="55" t="s">
+      <c r="H32" s="62" t="s">
         <v>137</v>
       </c>
-      <c r="I32" s="46" t="s">
+      <c r="I32" s="68" t="s">
         <v>138</v>
       </c>
-      <c r="J32" s="49" t="s">
+      <c r="J32" s="60" t="s">
         <v>86</v>
       </c>
-      <c r="K32" s="55" t="s">
+      <c r="K32" s="62" t="s">
         <v>102</v>
       </c>
-      <c r="L32" s="46" t="s">
+      <c r="L32" s="68" t="s">
         <v>88</v>
       </c>
       <c r="M32" s="14" t="s">
@@ -5184,17 +5208,17 @@
       </c>
     </row>
     <row r="33" spans="2:16" ht="24">
-      <c r="B33" s="50"/>
-      <c r="C33" s="50"/>
-      <c r="D33" s="50"/>
-      <c r="E33" s="50"/>
-      <c r="F33" s="59"/>
-      <c r="G33" s="50"/>
-      <c r="H33" s="56"/>
-      <c r="I33" s="47"/>
-      <c r="J33" s="50"/>
-      <c r="K33" s="56"/>
-      <c r="L33" s="47"/>
+      <c r="B33" s="66"/>
+      <c r="C33" s="66"/>
+      <c r="D33" s="66"/>
+      <c r="E33" s="66"/>
+      <c r="F33" s="67"/>
+      <c r="G33" s="66"/>
+      <c r="H33" s="69"/>
+      <c r="I33" s="70"/>
+      <c r="J33" s="66"/>
+      <c r="K33" s="69"/>
+      <c r="L33" s="70"/>
       <c r="M33" s="14" t="s">
         <v>104</v>
       </c>
@@ -5203,17 +5227,17 @@
       </c>
     </row>
     <row r="34" spans="2:16" ht="36">
-      <c r="B34" s="50"/>
-      <c r="C34" s="50"/>
-      <c r="D34" s="50"/>
-      <c r="E34" s="50"/>
-      <c r="F34" s="59"/>
-      <c r="G34" s="50"/>
-      <c r="H34" s="56"/>
-      <c r="I34" s="47"/>
-      <c r="J34" s="50"/>
-      <c r="K34" s="56"/>
-      <c r="L34" s="47"/>
+      <c r="B34" s="66"/>
+      <c r="C34" s="66"/>
+      <c r="D34" s="66"/>
+      <c r="E34" s="66"/>
+      <c r="F34" s="67"/>
+      <c r="G34" s="66"/>
+      <c r="H34" s="69"/>
+      <c r="I34" s="70"/>
+      <c r="J34" s="66"/>
+      <c r="K34" s="69"/>
+      <c r="L34" s="70"/>
       <c r="M34" s="14" t="s">
         <v>140</v>
       </c>
@@ -5225,51 +5249,51 @@
       </c>
     </row>
     <row r="35" spans="2:16" ht="24">
-      <c r="B35" s="50"/>
-      <c r="C35" s="50"/>
-      <c r="D35" s="50"/>
-      <c r="E35" s="50"/>
-      <c r="F35" s="59"/>
-      <c r="G35" s="50"/>
-      <c r="H35" s="56"/>
-      <c r="I35" s="47"/>
-      <c r="J35" s="50"/>
-      <c r="K35" s="56"/>
-      <c r="L35" s="47"/>
+      <c r="B35" s="66"/>
+      <c r="C35" s="66"/>
+      <c r="D35" s="66"/>
+      <c r="E35" s="66"/>
+      <c r="F35" s="67"/>
+      <c r="G35" s="66"/>
+      <c r="H35" s="69"/>
+      <c r="I35" s="70"/>
+      <c r="J35" s="66"/>
+      <c r="K35" s="69"/>
+      <c r="L35" s="70"/>
       <c r="M35" s="23" t="s">
         <v>141</v>
       </c>
       <c r="N35" s="22"/>
     </row>
     <row r="36" spans="2:16">
-      <c r="B36" s="50"/>
-      <c r="C36" s="50"/>
-      <c r="D36" s="50"/>
-      <c r="E36" s="50"/>
-      <c r="F36" s="59"/>
-      <c r="G36" s="50"/>
-      <c r="H36" s="56"/>
-      <c r="I36" s="47"/>
-      <c r="J36" s="50"/>
-      <c r="K36" s="56"/>
-      <c r="L36" s="47"/>
+      <c r="B36" s="66"/>
+      <c r="C36" s="66"/>
+      <c r="D36" s="66"/>
+      <c r="E36" s="66"/>
+      <c r="F36" s="67"/>
+      <c r="G36" s="66"/>
+      <c r="H36" s="69"/>
+      <c r="I36" s="70"/>
+      <c r="J36" s="66"/>
+      <c r="K36" s="69"/>
+      <c r="L36" s="70"/>
       <c r="M36" s="14" t="s">
         <v>142</v>
       </c>
       <c r="N36" s="22"/>
     </row>
     <row r="37" spans="2:16" ht="24">
-      <c r="B37" s="50"/>
-      <c r="C37" s="50"/>
-      <c r="D37" s="50"/>
-      <c r="E37" s="50"/>
-      <c r="F37" s="59"/>
-      <c r="G37" s="50"/>
-      <c r="H37" s="56"/>
-      <c r="I37" s="47"/>
-      <c r="J37" s="50"/>
-      <c r="K37" s="56"/>
-      <c r="L37" s="47"/>
+      <c r="B37" s="66"/>
+      <c r="C37" s="66"/>
+      <c r="D37" s="66"/>
+      <c r="E37" s="66"/>
+      <c r="F37" s="67"/>
+      <c r="G37" s="66"/>
+      <c r="H37" s="69"/>
+      <c r="I37" s="70"/>
+      <c r="J37" s="66"/>
+      <c r="K37" s="69"/>
+      <c r="L37" s="70"/>
       <c r="M37" s="37" t="s">
         <v>126</v>
       </c>
@@ -5280,50 +5304,50 @@
       <c r="C38" s="51"/>
       <c r="D38" s="51"/>
       <c r="E38" s="51"/>
-      <c r="F38" s="60"/>
+      <c r="F38" s="53"/>
       <c r="G38" s="51"/>
-      <c r="H38" s="57"/>
-      <c r="I38" s="48"/>
+      <c r="H38" s="59"/>
+      <c r="I38" s="57"/>
       <c r="J38" s="51"/>
-      <c r="K38" s="57"/>
-      <c r="L38" s="48"/>
+      <c r="K38" s="59"/>
+      <c r="L38" s="57"/>
       <c r="M38" s="21" t="s">
         <v>127</v>
       </c>
       <c r="N38" s="18"/>
     </row>
     <row r="39" spans="2:16" ht="24.75" thickTop="1">
-      <c r="B39" s="61" t="s">
-        <v>88</v>
-      </c>
-      <c r="C39" s="62">
+      <c r="B39" s="56" t="s">
+        <v>88</v>
+      </c>
+      <c r="C39" s="50">
         <v>8</v>
       </c>
-      <c r="D39" s="62">
+      <c r="D39" s="50">
         <v>11</v>
       </c>
-      <c r="E39" s="62">
+      <c r="E39" s="50">
         <v>11</v>
       </c>
-      <c r="F39" s="63">
+      <c r="F39" s="52">
         <v>11</v>
       </c>
-      <c r="G39" s="62">
+      <c r="G39" s="50">
         <v>11</v>
       </c>
-      <c r="H39" s="71" t="s">
+      <c r="H39" s="58" t="s">
         <v>144</v>
       </c>
-      <c r="I39" s="61" t="s">
+      <c r="I39" s="56" t="s">
         <v>145</v>
       </c>
-      <c r="J39" s="62" t="s">
+      <c r="J39" s="50" t="s">
         <v>86</v>
       </c>
-      <c r="K39" s="71" t="s">
+      <c r="K39" s="58" t="s">
         <v>102</v>
       </c>
-      <c r="L39" s="61" t="s">
+      <c r="L39" s="56" t="s">
         <v>88</v>
       </c>
       <c r="M39" s="14" t="s">
@@ -5334,17 +5358,17 @@
       </c>
     </row>
     <row r="40" spans="2:16" ht="24">
-      <c r="B40" s="47"/>
-      <c r="C40" s="50"/>
-      <c r="D40" s="50"/>
-      <c r="E40" s="50"/>
-      <c r="F40" s="59"/>
-      <c r="G40" s="50"/>
-      <c r="H40" s="56"/>
-      <c r="I40" s="47"/>
-      <c r="J40" s="50"/>
-      <c r="K40" s="56"/>
-      <c r="L40" s="47"/>
+      <c r="B40" s="70"/>
+      <c r="C40" s="66"/>
+      <c r="D40" s="66"/>
+      <c r="E40" s="66"/>
+      <c r="F40" s="67"/>
+      <c r="G40" s="66"/>
+      <c r="H40" s="69"/>
+      <c r="I40" s="70"/>
+      <c r="J40" s="66"/>
+      <c r="K40" s="69"/>
+      <c r="L40" s="70"/>
       <c r="M40" s="14" t="s">
         <v>116</v>
       </c>
@@ -5353,17 +5377,17 @@
       </c>
     </row>
     <row r="41" spans="2:16">
-      <c r="B41" s="47"/>
-      <c r="C41" s="50"/>
-      <c r="D41" s="50"/>
-      <c r="E41" s="50"/>
-      <c r="F41" s="59"/>
-      <c r="G41" s="50"/>
-      <c r="H41" s="56"/>
-      <c r="I41" s="47"/>
-      <c r="J41" s="50"/>
-      <c r="K41" s="56"/>
-      <c r="L41" s="47"/>
+      <c r="B41" s="70"/>
+      <c r="C41" s="66"/>
+      <c r="D41" s="66"/>
+      <c r="E41" s="66"/>
+      <c r="F41" s="67"/>
+      <c r="G41" s="66"/>
+      <c r="H41" s="69"/>
+      <c r="I41" s="70"/>
+      <c r="J41" s="66"/>
+      <c r="K41" s="69"/>
+      <c r="L41" s="70"/>
       <c r="M41" s="14" t="s">
         <v>142</v>
       </c>
@@ -5375,60 +5399,60 @@
       </c>
     </row>
     <row r="42" spans="2:16" ht="15" thickBot="1">
-      <c r="B42" s="48"/>
+      <c r="B42" s="57"/>
       <c r="C42" s="51"/>
       <c r="D42" s="51"/>
       <c r="E42" s="51"/>
-      <c r="F42" s="60"/>
+      <c r="F42" s="53"/>
       <c r="G42" s="51"/>
-      <c r="H42" s="57"/>
-      <c r="I42" s="48"/>
+      <c r="H42" s="59"/>
+      <c r="I42" s="57"/>
       <c r="J42" s="51"/>
-      <c r="K42" s="57"/>
-      <c r="L42" s="48"/>
+      <c r="K42" s="59"/>
+      <c r="L42" s="57"/>
       <c r="M42" s="19" t="s">
         <v>147</v>
       </c>
       <c r="N42" s="18"/>
     </row>
     <row r="43" spans="2:16">
-      <c r="B43" s="46" t="s">
-        <v>88</v>
-      </c>
-      <c r="C43" s="49">
+      <c r="B43" s="68" t="s">
+        <v>88</v>
+      </c>
+      <c r="C43" s="60">
         <v>9</v>
       </c>
-      <c r="D43" s="49">
+      <c r="D43" s="60">
         <v>12</v>
       </c>
-      <c r="E43" s="49">
+      <c r="E43" s="60">
         <v>12</v>
       </c>
-      <c r="F43" s="58">
+      <c r="F43" s="61">
         <v>12</v>
       </c>
-      <c r="G43" s="49">
+      <c r="G43" s="60">
         <v>12</v>
       </c>
-      <c r="H43" s="55" t="s">
+      <c r="H43" s="62" t="s">
         <v>149</v>
       </c>
-      <c r="I43" s="46" t="s">
+      <c r="I43" s="68" t="s">
         <v>150</v>
       </c>
-      <c r="J43" s="49" t="s">
+      <c r="J43" s="60" t="s">
         <v>86</v>
       </c>
-      <c r="K43" s="49" t="s">
+      <c r="K43" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="L43" s="46" t="s">
+      <c r="L43" s="68" t="s">
         <v>88</v>
       </c>
       <c r="M43" s="14" t="s">
         <v>151</v>
       </c>
-      <c r="N43" s="70" t="s">
+      <c r="N43" s="74" t="s">
         <v>154</v>
       </c>
       <c r="P43" t="s">
@@ -5436,143 +5460,143 @@
       </c>
     </row>
     <row r="44" spans="2:16" ht="24">
-      <c r="B44" s="47"/>
-      <c r="C44" s="50"/>
-      <c r="D44" s="50"/>
-      <c r="E44" s="50"/>
-      <c r="F44" s="59"/>
-      <c r="G44" s="50"/>
-      <c r="H44" s="56"/>
-      <c r="I44" s="47"/>
-      <c r="J44" s="50"/>
-      <c r="K44" s="50"/>
-      <c r="L44" s="47"/>
+      <c r="B44" s="70"/>
+      <c r="C44" s="66"/>
+      <c r="D44" s="66"/>
+      <c r="E44" s="66"/>
+      <c r="F44" s="67"/>
+      <c r="G44" s="66"/>
+      <c r="H44" s="69"/>
+      <c r="I44" s="70"/>
+      <c r="J44" s="66"/>
+      <c r="K44" s="66"/>
+      <c r="L44" s="70"/>
       <c r="M44" s="14" t="s">
         <v>152</v>
       </c>
-      <c r="N44" s="65"/>
+      <c r="N44" s="75"/>
     </row>
     <row r="45" spans="2:16" ht="24">
-      <c r="B45" s="47"/>
-      <c r="C45" s="50"/>
-      <c r="D45" s="50"/>
-      <c r="E45" s="50"/>
-      <c r="F45" s="59"/>
-      <c r="G45" s="50"/>
-      <c r="H45" s="56"/>
-      <c r="I45" s="47"/>
-      <c r="J45" s="50"/>
-      <c r="K45" s="50"/>
-      <c r="L45" s="47"/>
+      <c r="B45" s="70"/>
+      <c r="C45" s="66"/>
+      <c r="D45" s="66"/>
+      <c r="E45" s="66"/>
+      <c r="F45" s="67"/>
+      <c r="G45" s="66"/>
+      <c r="H45" s="69"/>
+      <c r="I45" s="70"/>
+      <c r="J45" s="66"/>
+      <c r="K45" s="66"/>
+      <c r="L45" s="70"/>
       <c r="M45" s="14" t="s">
         <v>153</v>
       </c>
-      <c r="N45" s="65"/>
+      <c r="N45" s="75"/>
     </row>
     <row r="46" spans="2:16" ht="24">
-      <c r="B46" s="47"/>
-      <c r="C46" s="50"/>
-      <c r="D46" s="50"/>
-      <c r="E46" s="50"/>
-      <c r="F46" s="59"/>
-      <c r="G46" s="50"/>
-      <c r="H46" s="56"/>
-      <c r="I46" s="47"/>
-      <c r="J46" s="50"/>
-      <c r="K46" s="50"/>
-      <c r="L46" s="47"/>
+      <c r="B46" s="70"/>
+      <c r="C46" s="66"/>
+      <c r="D46" s="66"/>
+      <c r="E46" s="66"/>
+      <c r="F46" s="67"/>
+      <c r="G46" s="66"/>
+      <c r="H46" s="69"/>
+      <c r="I46" s="70"/>
+      <c r="J46" s="66"/>
+      <c r="K46" s="66"/>
+      <c r="L46" s="70"/>
       <c r="M46" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="N46" s="65"/>
+      <c r="N46" s="75"/>
     </row>
     <row r="47" spans="2:16" ht="24.75" thickBot="1">
-      <c r="B47" s="48"/>
+      <c r="B47" s="57"/>
       <c r="C47" s="51"/>
       <c r="D47" s="51"/>
       <c r="E47" s="51"/>
-      <c r="F47" s="60"/>
+      <c r="F47" s="53"/>
       <c r="G47" s="51"/>
-      <c r="H47" s="57"/>
-      <c r="I47" s="48"/>
+      <c r="H47" s="59"/>
+      <c r="I47" s="57"/>
       <c r="J47" s="51"/>
       <c r="K47" s="51"/>
-      <c r="L47" s="48"/>
+      <c r="L47" s="57"/>
       <c r="M47" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="N47" s="66"/>
+      <c r="N47" s="76"/>
     </row>
     <row r="48" spans="2:16" ht="14.25" customHeight="1">
-      <c r="B48" s="49">
+      <c r="B48" s="60">
         <v>8</v>
       </c>
-      <c r="C48" s="49">
+      <c r="C48" s="60">
         <v>10</v>
       </c>
-      <c r="D48" s="49">
+      <c r="D48" s="60">
         <v>13</v>
       </c>
-      <c r="E48" s="49">
+      <c r="E48" s="60">
         <v>13</v>
       </c>
-      <c r="F48" s="58">
+      <c r="F48" s="61">
         <v>13</v>
       </c>
-      <c r="G48" s="49">
+      <c r="G48" s="60">
         <v>13</v>
       </c>
-      <c r="H48" s="55" t="s">
+      <c r="H48" s="62" t="s">
         <v>155</v>
       </c>
-      <c r="I48" s="46" t="s">
+      <c r="I48" s="68" t="s">
         <v>156</v>
       </c>
-      <c r="J48" s="49" t="s">
+      <c r="J48" s="60" t="s">
         <v>86</v>
       </c>
-      <c r="K48" s="49" t="s">
+      <c r="K48" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="L48" s="46" t="s">
+      <c r="L48" s="68" t="s">
         <v>88</v>
       </c>
       <c r="M48" s="14" t="s">
         <v>157</v>
       </c>
-      <c r="N48" s="46" t="s">
+      <c r="N48" s="68" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="49" spans="2:16" ht="24">
-      <c r="B49" s="50"/>
-      <c r="C49" s="50"/>
-      <c r="D49" s="50"/>
-      <c r="E49" s="50"/>
-      <c r="F49" s="59"/>
-      <c r="G49" s="50"/>
-      <c r="H49" s="56"/>
-      <c r="I49" s="47"/>
-      <c r="J49" s="50"/>
-      <c r="K49" s="50"/>
-      <c r="L49" s="47"/>
+      <c r="B49" s="66"/>
+      <c r="C49" s="66"/>
+      <c r="D49" s="66"/>
+      <c r="E49" s="66"/>
+      <c r="F49" s="67"/>
+      <c r="G49" s="66"/>
+      <c r="H49" s="69"/>
+      <c r="I49" s="70"/>
+      <c r="J49" s="66"/>
+      <c r="K49" s="66"/>
+      <c r="L49" s="70"/>
       <c r="M49" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="N49" s="47"/>
+      <c r="N49" s="70"/>
     </row>
     <row r="50" spans="2:16" ht="24">
-      <c r="B50" s="50"/>
-      <c r="C50" s="50"/>
-      <c r="D50" s="50"/>
-      <c r="E50" s="50"/>
-      <c r="F50" s="59"/>
-      <c r="G50" s="50"/>
-      <c r="H50" s="56"/>
-      <c r="I50" s="47"/>
-      <c r="J50" s="50"/>
-      <c r="K50" s="50"/>
-      <c r="L50" s="47"/>
+      <c r="B50" s="66"/>
+      <c r="C50" s="66"/>
+      <c r="D50" s="66"/>
+      <c r="E50" s="66"/>
+      <c r="F50" s="67"/>
+      <c r="G50" s="66"/>
+      <c r="H50" s="69"/>
+      <c r="I50" s="70"/>
+      <c r="J50" s="66"/>
+      <c r="K50" s="66"/>
+      <c r="L50" s="70"/>
       <c r="M50" s="14" t="s">
         <v>159</v>
       </c>
@@ -5584,34 +5608,34 @@
       </c>
     </row>
     <row r="51" spans="2:16" ht="24">
-      <c r="B51" s="50"/>
-      <c r="C51" s="50"/>
-      <c r="D51" s="50"/>
-      <c r="E51" s="50"/>
-      <c r="F51" s="59"/>
-      <c r="G51" s="50"/>
-      <c r="H51" s="56"/>
-      <c r="I51" s="47"/>
-      <c r="J51" s="50"/>
-      <c r="K51" s="50"/>
-      <c r="L51" s="47"/>
+      <c r="B51" s="66"/>
+      <c r="C51" s="66"/>
+      <c r="D51" s="66"/>
+      <c r="E51" s="66"/>
+      <c r="F51" s="67"/>
+      <c r="G51" s="66"/>
+      <c r="H51" s="69"/>
+      <c r="I51" s="70"/>
+      <c r="J51" s="66"/>
+      <c r="K51" s="66"/>
+      <c r="L51" s="70"/>
       <c r="M51" s="14" t="s">
         <v>120</v>
       </c>
       <c r="N51" s="26"/>
     </row>
     <row r="52" spans="2:16" ht="24">
-      <c r="B52" s="50"/>
-      <c r="C52" s="50"/>
-      <c r="D52" s="50"/>
-      <c r="E52" s="50"/>
-      <c r="F52" s="59"/>
-      <c r="G52" s="50"/>
-      <c r="H52" s="56"/>
-      <c r="I52" s="47"/>
-      <c r="J52" s="50"/>
-      <c r="K52" s="50"/>
-      <c r="L52" s="47"/>
+      <c r="B52" s="66"/>
+      <c r="C52" s="66"/>
+      <c r="D52" s="66"/>
+      <c r="E52" s="66"/>
+      <c r="F52" s="67"/>
+      <c r="G52" s="66"/>
+      <c r="H52" s="69"/>
+      <c r="I52" s="70"/>
+      <c r="J52" s="66"/>
+      <c r="K52" s="66"/>
+      <c r="L52" s="70"/>
       <c r="M52" s="14" t="s">
         <v>115</v>
       </c>
@@ -5622,50 +5646,50 @@
       <c r="C53" s="51"/>
       <c r="D53" s="51"/>
       <c r="E53" s="51"/>
-      <c r="F53" s="60"/>
+      <c r="F53" s="53"/>
       <c r="G53" s="51"/>
-      <c r="H53" s="57"/>
-      <c r="I53" s="48"/>
+      <c r="H53" s="59"/>
+      <c r="I53" s="57"/>
       <c r="J53" s="51"/>
       <c r="K53" s="51"/>
-      <c r="L53" s="48"/>
+      <c r="L53" s="57"/>
       <c r="M53" s="21" t="s">
         <v>127</v>
       </c>
       <c r="N53" s="24"/>
     </row>
     <row r="54" spans="2:16" ht="24">
-      <c r="B54" s="46" t="s">
-        <v>88</v>
-      </c>
-      <c r="C54" s="46" t="s">
-        <v>88</v>
-      </c>
-      <c r="D54" s="46" t="s">
-        <v>88</v>
-      </c>
-      <c r="E54" s="49">
+      <c r="B54" s="68" t="s">
+        <v>88</v>
+      </c>
+      <c r="C54" s="68" t="s">
+        <v>88</v>
+      </c>
+      <c r="D54" s="68" t="s">
+        <v>88</v>
+      </c>
+      <c r="E54" s="60">
         <v>14</v>
       </c>
-      <c r="F54" s="58">
+      <c r="F54" s="61">
         <v>14</v>
       </c>
-      <c r="G54" s="49">
+      <c r="G54" s="60">
         <v>14</v>
       </c>
-      <c r="H54" s="55" t="s">
+      <c r="H54" s="62" t="s">
         <v>160</v>
       </c>
-      <c r="I54" s="70" t="s">
+      <c r="I54" s="74" t="s">
         <v>161</v>
       </c>
-      <c r="J54" s="49" t="s">
+      <c r="J54" s="60" t="s">
         <v>86</v>
       </c>
-      <c r="K54" s="49" t="s">
+      <c r="K54" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="L54" s="46" t="s">
+      <c r="L54" s="68" t="s">
         <v>88</v>
       </c>
       <c r="M54" s="14" t="s">
@@ -5679,17 +5703,17 @@
       </c>
     </row>
     <row r="55" spans="2:16">
-      <c r="B55" s="47"/>
-      <c r="C55" s="47"/>
-      <c r="D55" s="47"/>
-      <c r="E55" s="50"/>
-      <c r="F55" s="59"/>
-      <c r="G55" s="50"/>
-      <c r="H55" s="56"/>
-      <c r="I55" s="65"/>
-      <c r="J55" s="50"/>
-      <c r="K55" s="50"/>
-      <c r="L55" s="47"/>
+      <c r="B55" s="70"/>
+      <c r="C55" s="70"/>
+      <c r="D55" s="70"/>
+      <c r="E55" s="66"/>
+      <c r="F55" s="67"/>
+      <c r="G55" s="66"/>
+      <c r="H55" s="69"/>
+      <c r="I55" s="75"/>
+      <c r="J55" s="66"/>
+      <c r="K55" s="66"/>
+      <c r="L55" s="70"/>
       <c r="M55" s="14" t="s">
         <v>151</v>
       </c>
@@ -5698,88 +5722,88 @@
       </c>
     </row>
     <row r="56" spans="2:16">
-      <c r="B56" s="47"/>
-      <c r="C56" s="47"/>
-      <c r="D56" s="47"/>
-      <c r="E56" s="50"/>
-      <c r="F56" s="59"/>
-      <c r="G56" s="50"/>
-      <c r="H56" s="56"/>
-      <c r="I56" s="65"/>
-      <c r="J56" s="50"/>
-      <c r="K56" s="50"/>
-      <c r="L56" s="47"/>
+      <c r="B56" s="70"/>
+      <c r="C56" s="70"/>
+      <c r="D56" s="70"/>
+      <c r="E56" s="66"/>
+      <c r="F56" s="67"/>
+      <c r="G56" s="66"/>
+      <c r="H56" s="69"/>
+      <c r="I56" s="75"/>
+      <c r="J56" s="66"/>
+      <c r="K56" s="66"/>
+      <c r="L56" s="70"/>
       <c r="M56" s="14" t="s">
         <v>117</v>
       </c>
       <c r="N56" s="22"/>
     </row>
     <row r="57" spans="2:16" ht="24">
-      <c r="B57" s="47"/>
-      <c r="C57" s="47"/>
-      <c r="D57" s="47"/>
-      <c r="E57" s="50"/>
-      <c r="F57" s="59"/>
-      <c r="G57" s="50"/>
-      <c r="H57" s="56"/>
-      <c r="I57" s="65"/>
-      <c r="J57" s="50"/>
-      <c r="K57" s="50"/>
-      <c r="L57" s="47"/>
+      <c r="B57" s="70"/>
+      <c r="C57" s="70"/>
+      <c r="D57" s="70"/>
+      <c r="E57" s="66"/>
+      <c r="F57" s="67"/>
+      <c r="G57" s="66"/>
+      <c r="H57" s="69"/>
+      <c r="I57" s="75"/>
+      <c r="J57" s="66"/>
+      <c r="K57" s="66"/>
+      <c r="L57" s="70"/>
       <c r="M57" s="13" t="s">
         <v>119</v>
       </c>
       <c r="N57" s="22"/>
     </row>
     <row r="58" spans="2:16" ht="15" thickBot="1">
-      <c r="B58" s="48"/>
-      <c r="C58" s="48"/>
-      <c r="D58" s="48"/>
+      <c r="B58" s="57"/>
+      <c r="C58" s="57"/>
+      <c r="D58" s="57"/>
       <c r="E58" s="51"/>
-      <c r="F58" s="60"/>
+      <c r="F58" s="53"/>
       <c r="G58" s="51"/>
-      <c r="H58" s="57"/>
-      <c r="I58" s="66"/>
+      <c r="H58" s="59"/>
+      <c r="I58" s="76"/>
       <c r="J58" s="51"/>
       <c r="K58" s="51"/>
-      <c r="L58" s="48"/>
+      <c r="L58" s="57"/>
       <c r="M58" s="19" t="s">
         <v>162</v>
       </c>
       <c r="N58" s="18"/>
     </row>
     <row r="59" spans="2:16" ht="24">
-      <c r="B59" s="46" t="s">
-        <v>88</v>
-      </c>
-      <c r="C59" s="49">
+      <c r="B59" s="68" t="s">
+        <v>88</v>
+      </c>
+      <c r="C59" s="60">
         <v>11</v>
       </c>
-      <c r="D59" s="49">
+      <c r="D59" s="60">
         <v>14</v>
       </c>
-      <c r="E59" s="49">
+      <c r="E59" s="60">
         <v>15</v>
       </c>
-      <c r="F59" s="58">
+      <c r="F59" s="61">
         <v>15</v>
       </c>
-      <c r="G59" s="49">
+      <c r="G59" s="60">
         <v>15</v>
       </c>
-      <c r="H59" s="55" t="s">
+      <c r="H59" s="62" t="s">
         <v>165</v>
       </c>
-      <c r="I59" s="70" t="s">
+      <c r="I59" s="74" t="s">
         <v>166</v>
       </c>
-      <c r="J59" s="49" t="s">
+      <c r="J59" s="60" t="s">
         <v>86</v>
       </c>
-      <c r="K59" s="49" t="s">
+      <c r="K59" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="L59" s="46" t="s">
+      <c r="L59" s="68" t="s">
         <v>88</v>
       </c>
       <c r="M59" s="14" t="s">
@@ -5793,17 +5817,17 @@
       </c>
     </row>
     <row r="60" spans="2:16">
-      <c r="B60" s="47"/>
-      <c r="C60" s="50"/>
-      <c r="D60" s="50"/>
-      <c r="E60" s="50"/>
-      <c r="F60" s="59"/>
-      <c r="G60" s="50"/>
-      <c r="H60" s="56"/>
-      <c r="I60" s="65"/>
-      <c r="J60" s="50"/>
-      <c r="K60" s="50"/>
-      <c r="L60" s="47"/>
+      <c r="B60" s="70"/>
+      <c r="C60" s="66"/>
+      <c r="D60" s="66"/>
+      <c r="E60" s="66"/>
+      <c r="F60" s="67"/>
+      <c r="G60" s="66"/>
+      <c r="H60" s="69"/>
+      <c r="I60" s="75"/>
+      <c r="J60" s="66"/>
+      <c r="K60" s="66"/>
+      <c r="L60" s="70"/>
       <c r="M60" s="14" t="s">
         <v>157</v>
       </c>
@@ -5812,51 +5836,51 @@
       </c>
     </row>
     <row r="61" spans="2:16" ht="24">
-      <c r="B61" s="47"/>
-      <c r="C61" s="50"/>
-      <c r="D61" s="50"/>
-      <c r="E61" s="50"/>
-      <c r="F61" s="59"/>
-      <c r="G61" s="50"/>
-      <c r="H61" s="56"/>
-      <c r="I61" s="65"/>
-      <c r="J61" s="50"/>
-      <c r="K61" s="50"/>
-      <c r="L61" s="47"/>
+      <c r="B61" s="70"/>
+      <c r="C61" s="66"/>
+      <c r="D61" s="66"/>
+      <c r="E61" s="66"/>
+      <c r="F61" s="67"/>
+      <c r="G61" s="66"/>
+      <c r="H61" s="69"/>
+      <c r="I61" s="75"/>
+      <c r="J61" s="66"/>
+      <c r="K61" s="66"/>
+      <c r="L61" s="70"/>
       <c r="M61" s="14" t="s">
         <v>104</v>
       </c>
       <c r="N61" s="22"/>
     </row>
     <row r="62" spans="2:16" ht="24">
-      <c r="B62" s="47"/>
-      <c r="C62" s="50"/>
-      <c r="D62" s="50"/>
-      <c r="E62" s="50"/>
-      <c r="F62" s="59"/>
-      <c r="G62" s="50"/>
-      <c r="H62" s="56"/>
-      <c r="I62" s="65"/>
-      <c r="J62" s="50"/>
-      <c r="K62" s="50"/>
-      <c r="L62" s="47"/>
+      <c r="B62" s="70"/>
+      <c r="C62" s="66"/>
+      <c r="D62" s="66"/>
+      <c r="E62" s="66"/>
+      <c r="F62" s="67"/>
+      <c r="G62" s="66"/>
+      <c r="H62" s="69"/>
+      <c r="I62" s="75"/>
+      <c r="J62" s="66"/>
+      <c r="K62" s="66"/>
+      <c r="L62" s="70"/>
       <c r="M62" s="13" t="s">
         <v>167</v>
       </c>
       <c r="N62" s="22"/>
     </row>
     <row r="63" spans="2:16" ht="15" thickBot="1">
-      <c r="B63" s="48"/>
+      <c r="B63" s="57"/>
       <c r="C63" s="51"/>
       <c r="D63" s="51"/>
       <c r="E63" s="51"/>
-      <c r="F63" s="60"/>
+      <c r="F63" s="53"/>
       <c r="G63" s="51"/>
-      <c r="H63" s="57"/>
-      <c r="I63" s="66"/>
+      <c r="H63" s="59"/>
+      <c r="I63" s="76"/>
       <c r="J63" s="51"/>
       <c r="K63" s="51"/>
-      <c r="L63" s="48"/>
+      <c r="L63" s="57"/>
       <c r="M63" s="19" t="s">
         <v>168</v>
       </c>
@@ -5986,43 +6010,43 @@
       </c>
     </row>
     <row r="67" spans="2:16" ht="36">
-      <c r="B67" s="46" t="s">
-        <v>88</v>
-      </c>
-      <c r="C67" s="46" t="s">
-        <v>88</v>
-      </c>
-      <c r="D67" s="46" t="s">
-        <v>88</v>
-      </c>
-      <c r="E67" s="49">
+      <c r="B67" s="68" t="s">
+        <v>88</v>
+      </c>
+      <c r="C67" s="68" t="s">
+        <v>88</v>
+      </c>
+      <c r="D67" s="68" t="s">
+        <v>88</v>
+      </c>
+      <c r="E67" s="60">
         <v>18</v>
       </c>
-      <c r="F67" s="58">
+      <c r="F67" s="61">
         <v>18</v>
       </c>
-      <c r="G67" s="49">
+      <c r="G67" s="60">
         <v>18</v>
       </c>
-      <c r="H67" s="55" t="s">
+      <c r="H67" s="62" t="s">
         <v>176</v>
       </c>
-      <c r="I67" s="70" t="s">
+      <c r="I67" s="74" t="s">
         <v>177</v>
       </c>
-      <c r="J67" s="49" t="s">
+      <c r="J67" s="60" t="s">
         <v>86</v>
       </c>
-      <c r="K67" s="49" t="s">
+      <c r="K67" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="L67" s="46" t="s">
+      <c r="L67" s="68" t="s">
         <v>88</v>
       </c>
       <c r="M67" s="13" t="s">
         <v>178</v>
       </c>
-      <c r="N67" s="46" t="s">
+      <c r="N67" s="68" t="s">
         <v>88</v>
       </c>
       <c r="P67" t="s">
@@ -6030,860 +6054,860 @@
       </c>
     </row>
     <row r="68" spans="2:16" ht="24">
-      <c r="B68" s="47"/>
-      <c r="C68" s="47"/>
-      <c r="D68" s="47"/>
-      <c r="E68" s="50"/>
-      <c r="F68" s="59"/>
-      <c r="G68" s="50"/>
-      <c r="H68" s="56"/>
-      <c r="I68" s="65"/>
-      <c r="J68" s="50"/>
-      <c r="K68" s="50"/>
-      <c r="L68" s="47"/>
+      <c r="B68" s="70"/>
+      <c r="C68" s="70"/>
+      <c r="D68" s="70"/>
+      <c r="E68" s="66"/>
+      <c r="F68" s="67"/>
+      <c r="G68" s="66"/>
+      <c r="H68" s="69"/>
+      <c r="I68" s="75"/>
+      <c r="J68" s="66"/>
+      <c r="K68" s="66"/>
+      <c r="L68" s="70"/>
       <c r="M68" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="N68" s="47"/>
+      <c r="N68" s="70"/>
     </row>
     <row r="69" spans="2:16" ht="24">
-      <c r="B69" s="47"/>
-      <c r="C69" s="47"/>
-      <c r="D69" s="47"/>
-      <c r="E69" s="50"/>
-      <c r="F69" s="59"/>
-      <c r="G69" s="50"/>
-      <c r="H69" s="56"/>
-      <c r="I69" s="65"/>
-      <c r="J69" s="50"/>
-      <c r="K69" s="50"/>
-      <c r="L69" s="47"/>
+      <c r="B69" s="70"/>
+      <c r="C69" s="70"/>
+      <c r="D69" s="70"/>
+      <c r="E69" s="66"/>
+      <c r="F69" s="67"/>
+      <c r="G69" s="66"/>
+      <c r="H69" s="69"/>
+      <c r="I69" s="75"/>
+      <c r="J69" s="66"/>
+      <c r="K69" s="66"/>
+      <c r="L69" s="70"/>
       <c r="M69" s="14" t="s">
         <v>141</v>
       </c>
-      <c r="N69" s="47"/>
+      <c r="N69" s="70"/>
     </row>
     <row r="70" spans="2:16" ht="15" thickBot="1">
-      <c r="B70" s="48"/>
-      <c r="C70" s="48"/>
-      <c r="D70" s="48"/>
+      <c r="B70" s="57"/>
+      <c r="C70" s="57"/>
+      <c r="D70" s="57"/>
       <c r="E70" s="51"/>
-      <c r="F70" s="60"/>
+      <c r="F70" s="53"/>
       <c r="G70" s="51"/>
-      <c r="H70" s="57"/>
-      <c r="I70" s="66"/>
+      <c r="H70" s="59"/>
+      <c r="I70" s="76"/>
       <c r="J70" s="51"/>
       <c r="K70" s="51"/>
-      <c r="L70" s="48"/>
+      <c r="L70" s="57"/>
       <c r="M70" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="N70" s="48"/>
+      <c r="N70" s="57"/>
     </row>
     <row r="71" spans="2:16" ht="24">
-      <c r="B71" s="49">
+      <c r="B71" s="60">
         <v>11</v>
       </c>
-      <c r="C71" s="49">
+      <c r="C71" s="60">
         <v>14</v>
       </c>
-      <c r="D71" s="49">
+      <c r="D71" s="60">
         <v>17</v>
       </c>
-      <c r="E71" s="49">
+      <c r="E71" s="60">
         <v>19</v>
       </c>
-      <c r="F71" s="58">
+      <c r="F71" s="61">
         <v>19</v>
       </c>
-      <c r="G71" s="49">
+      <c r="G71" s="60">
         <v>19</v>
       </c>
-      <c r="H71" s="55" t="s">
+      <c r="H71" s="62" t="s">
         <v>179</v>
       </c>
-      <c r="I71" s="46" t="s">
+      <c r="I71" s="68" t="s">
         <v>180</v>
       </c>
-      <c r="J71" s="49" t="s">
+      <c r="J71" s="60" t="s">
         <v>86</v>
       </c>
-      <c r="K71" s="49" t="s">
+      <c r="K71" s="60" t="s">
         <v>181</v>
       </c>
-      <c r="L71" s="46" t="s">
+      <c r="L71" s="68" t="s">
         <v>88</v>
       </c>
       <c r="M71" s="12" t="s">
         <v>182</v>
       </c>
-      <c r="N71" s="46" t="s">
+      <c r="N71" s="68" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="72" spans="2:16" ht="24">
-      <c r="B72" s="50"/>
-      <c r="C72" s="50"/>
-      <c r="D72" s="50"/>
-      <c r="E72" s="50"/>
-      <c r="F72" s="59"/>
-      <c r="G72" s="50"/>
-      <c r="H72" s="56"/>
-      <c r="I72" s="47"/>
-      <c r="J72" s="50"/>
-      <c r="K72" s="50"/>
-      <c r="L72" s="47"/>
+      <c r="B72" s="66"/>
+      <c r="C72" s="66"/>
+      <c r="D72" s="66"/>
+      <c r="E72" s="66"/>
+      <c r="F72" s="67"/>
+      <c r="G72" s="66"/>
+      <c r="H72" s="69"/>
+      <c r="I72" s="70"/>
+      <c r="J72" s="66"/>
+      <c r="K72" s="66"/>
+      <c r="L72" s="70"/>
       <c r="M72" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="N72" s="47"/>
+      <c r="N72" s="70"/>
     </row>
     <row r="73" spans="2:16" ht="24">
-      <c r="B73" s="50"/>
-      <c r="C73" s="50"/>
-      <c r="D73" s="50"/>
-      <c r="E73" s="50"/>
-      <c r="F73" s="59"/>
-      <c r="G73" s="50"/>
-      <c r="H73" s="56"/>
-      <c r="I73" s="47"/>
-      <c r="J73" s="50"/>
-      <c r="K73" s="50"/>
-      <c r="L73" s="47"/>
+      <c r="B73" s="66"/>
+      <c r="C73" s="66"/>
+      <c r="D73" s="66"/>
+      <c r="E73" s="66"/>
+      <c r="F73" s="67"/>
+      <c r="G73" s="66"/>
+      <c r="H73" s="69"/>
+      <c r="I73" s="70"/>
+      <c r="J73" s="66"/>
+      <c r="K73" s="66"/>
+      <c r="L73" s="70"/>
       <c r="M73" s="38" t="s">
         <v>125</v>
       </c>
-      <c r="N73" s="47"/>
+      <c r="N73" s="70"/>
     </row>
     <row r="74" spans="2:16" ht="48.75" thickBot="1">
       <c r="B74" s="51"/>
       <c r="C74" s="51"/>
       <c r="D74" s="51"/>
       <c r="E74" s="51"/>
-      <c r="F74" s="60"/>
+      <c r="F74" s="53"/>
       <c r="G74" s="51"/>
-      <c r="H74" s="57"/>
-      <c r="I74" s="48"/>
+      <c r="H74" s="59"/>
+      <c r="I74" s="57"/>
       <c r="J74" s="51"/>
       <c r="K74" s="51"/>
-      <c r="L74" s="48"/>
+      <c r="L74" s="57"/>
       <c r="M74" s="19" t="s">
         <v>183</v>
       </c>
-      <c r="N74" s="48"/>
+      <c r="N74" s="57"/>
     </row>
     <row r="75" spans="2:16" ht="36.75" thickTop="1">
-      <c r="B75" s="62">
+      <c r="B75" s="50">
         <v>12</v>
       </c>
-      <c r="C75" s="62">
+      <c r="C75" s="50">
         <v>15</v>
       </c>
-      <c r="D75" s="62">
+      <c r="D75" s="50">
         <v>18</v>
       </c>
-      <c r="E75" s="62">
+      <c r="E75" s="50">
         <v>20</v>
       </c>
-      <c r="F75" s="63">
+      <c r="F75" s="52">
         <v>20</v>
       </c>
-      <c r="G75" s="62">
+      <c r="G75" s="50">
         <v>20</v>
       </c>
-      <c r="H75" s="71" t="s">
+      <c r="H75" s="58" t="s">
         <v>184</v>
       </c>
-      <c r="I75" s="61" t="s">
+      <c r="I75" s="56" t="s">
         <v>185</v>
       </c>
-      <c r="J75" s="62" t="s">
+      <c r="J75" s="50" t="s">
         <v>86</v>
       </c>
-      <c r="K75" s="62" t="s">
+      <c r="K75" s="50" t="s">
         <v>181</v>
       </c>
-      <c r="L75" s="72">
+      <c r="L75" s="77">
         <v>-7</v>
       </c>
       <c r="M75" s="14" t="s">
         <v>186</v>
       </c>
-      <c r="N75" s="61" t="s">
+      <c r="N75" s="56" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="76" spans="2:16" ht="24">
-      <c r="B76" s="50"/>
-      <c r="C76" s="50"/>
-      <c r="D76" s="50"/>
-      <c r="E76" s="50"/>
-      <c r="F76" s="59"/>
-      <c r="G76" s="50"/>
-      <c r="H76" s="56"/>
-      <c r="I76" s="47"/>
-      <c r="J76" s="50"/>
-      <c r="K76" s="50"/>
-      <c r="L76" s="68"/>
+      <c r="B76" s="66"/>
+      <c r="C76" s="66"/>
+      <c r="D76" s="66"/>
+      <c r="E76" s="66"/>
+      <c r="F76" s="67"/>
+      <c r="G76" s="66"/>
+      <c r="H76" s="69"/>
+      <c r="I76" s="70"/>
+      <c r="J76" s="66"/>
+      <c r="K76" s="66"/>
+      <c r="L76" s="78"/>
       <c r="M76" s="14" t="s">
         <v>187</v>
       </c>
-      <c r="N76" s="47"/>
+      <c r="N76" s="70"/>
     </row>
     <row r="77" spans="2:16" ht="24">
-      <c r="B77" s="50"/>
-      <c r="C77" s="50"/>
-      <c r="D77" s="50"/>
-      <c r="E77" s="50"/>
-      <c r="F77" s="59"/>
-      <c r="G77" s="50"/>
-      <c r="H77" s="56"/>
-      <c r="I77" s="47"/>
-      <c r="J77" s="50"/>
-      <c r="K77" s="50"/>
-      <c r="L77" s="68"/>
+      <c r="B77" s="66"/>
+      <c r="C77" s="66"/>
+      <c r="D77" s="66"/>
+      <c r="E77" s="66"/>
+      <c r="F77" s="67"/>
+      <c r="G77" s="66"/>
+      <c r="H77" s="69"/>
+      <c r="I77" s="70"/>
+      <c r="J77" s="66"/>
+      <c r="K77" s="66"/>
+      <c r="L77" s="78"/>
       <c r="M77" s="38" t="s">
         <v>103</v>
       </c>
-      <c r="N77" s="47"/>
+      <c r="N77" s="70"/>
     </row>
     <row r="78" spans="2:16">
-      <c r="B78" s="50"/>
-      <c r="C78" s="50"/>
-      <c r="D78" s="50"/>
-      <c r="E78" s="50"/>
-      <c r="F78" s="59"/>
-      <c r="G78" s="50"/>
-      <c r="H78" s="56"/>
-      <c r="I78" s="47"/>
-      <c r="J78" s="50"/>
-      <c r="K78" s="50"/>
-      <c r="L78" s="68"/>
+      <c r="B78" s="66"/>
+      <c r="C78" s="66"/>
+      <c r="D78" s="66"/>
+      <c r="E78" s="66"/>
+      <c r="F78" s="67"/>
+      <c r="G78" s="66"/>
+      <c r="H78" s="69"/>
+      <c r="I78" s="70"/>
+      <c r="J78" s="66"/>
+      <c r="K78" s="66"/>
+      <c r="L78" s="78"/>
       <c r="M78" s="14" t="s">
         <v>188</v>
       </c>
-      <c r="N78" s="47"/>
+      <c r="N78" s="70"/>
     </row>
     <row r="79" spans="2:16" ht="24.75" thickBot="1">
       <c r="B79" s="51"/>
       <c r="C79" s="51"/>
       <c r="D79" s="51"/>
       <c r="E79" s="51"/>
-      <c r="F79" s="60"/>
+      <c r="F79" s="53"/>
       <c r="G79" s="51"/>
-      <c r="H79" s="57"/>
-      <c r="I79" s="48"/>
+      <c r="H79" s="59"/>
+      <c r="I79" s="57"/>
       <c r="J79" s="51"/>
       <c r="K79" s="51"/>
-      <c r="L79" s="69"/>
+      <c r="L79" s="79"/>
       <c r="M79" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="N79" s="48"/>
+      <c r="N79" s="57"/>
     </row>
     <row r="80" spans="2:16">
-      <c r="B80" s="46" t="s">
-        <v>88</v>
-      </c>
-      <c r="C80" s="46" t="s">
-        <v>88</v>
-      </c>
-      <c r="D80" s="46" t="s">
-        <v>88</v>
-      </c>
-      <c r="E80" s="46" t="s">
-        <v>88</v>
-      </c>
-      <c r="F80" s="58">
+      <c r="B80" s="68" t="s">
+        <v>88</v>
+      </c>
+      <c r="C80" s="68" t="s">
+        <v>88</v>
+      </c>
+      <c r="D80" s="68" t="s">
+        <v>88</v>
+      </c>
+      <c r="E80" s="68" t="s">
+        <v>88</v>
+      </c>
+      <c r="F80" s="61">
         <v>21</v>
       </c>
-      <c r="G80" s="49">
+      <c r="G80" s="60">
         <v>21</v>
       </c>
-      <c r="H80" s="46" t="s">
-        <v>88</v>
-      </c>
-      <c r="I80" s="46" t="s">
+      <c r="H80" s="68" t="s">
+        <v>88</v>
+      </c>
+      <c r="I80" s="68" t="s">
         <v>189</v>
       </c>
-      <c r="J80" s="49" t="s">
+      <c r="J80" s="60" t="s">
         <v>86</v>
       </c>
-      <c r="K80" s="49" t="s">
+      <c r="K80" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="L80" s="46" t="s">
+      <c r="L80" s="68" t="s">
         <v>88</v>
       </c>
       <c r="M80" s="14" t="s">
         <v>151</v>
       </c>
-      <c r="N80" s="46" t="s">
+      <c r="N80" s="68" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="81" spans="2:19" ht="48">
-      <c r="B81" s="47"/>
-      <c r="C81" s="47"/>
-      <c r="D81" s="47"/>
-      <c r="E81" s="47"/>
-      <c r="F81" s="59"/>
-      <c r="G81" s="50"/>
-      <c r="H81" s="47"/>
-      <c r="I81" s="47"/>
-      <c r="J81" s="50"/>
-      <c r="K81" s="50"/>
-      <c r="L81" s="47"/>
+      <c r="B81" s="70"/>
+      <c r="C81" s="70"/>
+      <c r="D81" s="70"/>
+      <c r="E81" s="70"/>
+      <c r="F81" s="67"/>
+      <c r="G81" s="66"/>
+      <c r="H81" s="70"/>
+      <c r="I81" s="70"/>
+      <c r="J81" s="66"/>
+      <c r="K81" s="66"/>
+      <c r="L81" s="70"/>
       <c r="M81" s="14" t="s">
         <v>190</v>
       </c>
-      <c r="N81" s="47"/>
+      <c r="N81" s="70"/>
     </row>
     <row r="82" spans="2:19" ht="24">
-      <c r="B82" s="47"/>
-      <c r="C82" s="47"/>
-      <c r="D82" s="47"/>
-      <c r="E82" s="47"/>
-      <c r="F82" s="59"/>
-      <c r="G82" s="50"/>
-      <c r="H82" s="47"/>
-      <c r="I82" s="47"/>
-      <c r="J82" s="50"/>
-      <c r="K82" s="50"/>
-      <c r="L82" s="47"/>
+      <c r="B82" s="70"/>
+      <c r="C82" s="70"/>
+      <c r="D82" s="70"/>
+      <c r="E82" s="70"/>
+      <c r="F82" s="67"/>
+      <c r="G82" s="66"/>
+      <c r="H82" s="70"/>
+      <c r="I82" s="70"/>
+      <c r="J82" s="66"/>
+      <c r="K82" s="66"/>
+      <c r="L82" s="70"/>
       <c r="M82" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="N82" s="47"/>
+      <c r="N82" s="70"/>
     </row>
     <row r="83" spans="2:19" ht="48.75" thickBot="1">
-      <c r="B83" s="48"/>
-      <c r="C83" s="48"/>
-      <c r="D83" s="48"/>
-      <c r="E83" s="48"/>
-      <c r="F83" s="60"/>
+      <c r="B83" s="57"/>
+      <c r="C83" s="57"/>
+      <c r="D83" s="57"/>
+      <c r="E83" s="57"/>
+      <c r="F83" s="53"/>
       <c r="G83" s="51"/>
-      <c r="H83" s="48"/>
-      <c r="I83" s="48"/>
+      <c r="H83" s="57"/>
+      <c r="I83" s="57"/>
       <c r="J83" s="51"/>
       <c r="K83" s="51"/>
-      <c r="L83" s="48"/>
+      <c r="L83" s="57"/>
       <c r="M83" s="19" t="s">
         <v>183</v>
       </c>
-      <c r="N83" s="48"/>
+      <c r="N83" s="57"/>
     </row>
     <row r="84" spans="2:19">
-      <c r="B84" s="46" t="s">
-        <v>88</v>
-      </c>
-      <c r="C84" s="46" t="s">
-        <v>88</v>
-      </c>
-      <c r="D84" s="46" t="s">
-        <v>88</v>
-      </c>
-      <c r="E84" s="46" t="s">
-        <v>88</v>
-      </c>
-      <c r="F84" s="58">
+      <c r="B84" s="68" t="s">
+        <v>88</v>
+      </c>
+      <c r="C84" s="68" t="s">
+        <v>88</v>
+      </c>
+      <c r="D84" s="68" t="s">
+        <v>88</v>
+      </c>
+      <c r="E84" s="68" t="s">
+        <v>88</v>
+      </c>
+      <c r="F84" s="61">
         <v>22</v>
       </c>
-      <c r="G84" s="49">
+      <c r="G84" s="60">
         <v>22</v>
       </c>
-      <c r="H84" s="46" t="s">
-        <v>88</v>
-      </c>
-      <c r="I84" s="46" t="s">
+      <c r="H84" s="68" t="s">
+        <v>88</v>
+      </c>
+      <c r="I84" s="68" t="s">
         <v>191</v>
       </c>
-      <c r="J84" s="49" t="s">
+      <c r="J84" s="60" t="s">
         <v>86</v>
       </c>
-      <c r="K84" s="49" t="s">
+      <c r="K84" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="L84" s="46" t="s">
+      <c r="L84" s="68" t="s">
         <v>88</v>
       </c>
       <c r="M84" s="14" t="s">
         <v>157</v>
       </c>
-      <c r="N84" s="46" t="s">
+      <c r="N84" s="68" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="85" spans="2:19" ht="24">
-      <c r="B85" s="47"/>
-      <c r="C85" s="47"/>
-      <c r="D85" s="47"/>
-      <c r="E85" s="47"/>
-      <c r="F85" s="59"/>
-      <c r="G85" s="50"/>
-      <c r="H85" s="47"/>
-      <c r="I85" s="47"/>
-      <c r="J85" s="50"/>
-      <c r="K85" s="50"/>
-      <c r="L85" s="47"/>
+      <c r="B85" s="70"/>
+      <c r="C85" s="70"/>
+      <c r="D85" s="70"/>
+      <c r="E85" s="70"/>
+      <c r="F85" s="67"/>
+      <c r="G85" s="66"/>
+      <c r="H85" s="70"/>
+      <c r="I85" s="70"/>
+      <c r="J85" s="66"/>
+      <c r="K85" s="66"/>
+      <c r="L85" s="70"/>
       <c r="M85" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="N85" s="47"/>
+      <c r="N85" s="70"/>
     </row>
     <row r="86" spans="2:19" ht="24">
-      <c r="B86" s="47"/>
-      <c r="C86" s="47"/>
-      <c r="D86" s="47"/>
-      <c r="E86" s="47"/>
-      <c r="F86" s="59"/>
-      <c r="G86" s="50"/>
-      <c r="H86" s="47"/>
-      <c r="I86" s="47"/>
-      <c r="J86" s="50"/>
-      <c r="K86" s="50"/>
-      <c r="L86" s="47"/>
+      <c r="B86" s="70"/>
+      <c r="C86" s="70"/>
+      <c r="D86" s="70"/>
+      <c r="E86" s="70"/>
+      <c r="F86" s="67"/>
+      <c r="G86" s="66"/>
+      <c r="H86" s="70"/>
+      <c r="I86" s="70"/>
+      <c r="J86" s="66"/>
+      <c r="K86" s="66"/>
+      <c r="L86" s="70"/>
       <c r="M86" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="N86" s="47"/>
+      <c r="N86" s="70"/>
       <c r="S86" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="87" spans="2:19" ht="24.75" thickBot="1">
-      <c r="B87" s="48"/>
-      <c r="C87" s="48"/>
-      <c r="D87" s="48"/>
-      <c r="E87" s="48"/>
-      <c r="F87" s="60"/>
+      <c r="B87" s="57"/>
+      <c r="C87" s="57"/>
+      <c r="D87" s="57"/>
+      <c r="E87" s="57"/>
+      <c r="F87" s="53"/>
       <c r="G87" s="51"/>
-      <c r="H87" s="48"/>
-      <c r="I87" s="48"/>
+      <c r="H87" s="57"/>
+      <c r="I87" s="57"/>
       <c r="J87" s="51"/>
       <c r="K87" s="51"/>
-      <c r="L87" s="48"/>
+      <c r="L87" s="57"/>
       <c r="M87" s="19" t="s">
         <v>127</v>
       </c>
-      <c r="N87" s="48"/>
+      <c r="N87" s="57"/>
     </row>
     <row r="88" spans="2:19">
-      <c r="B88" s="49">
+      <c r="B88" s="60">
         <v>13</v>
       </c>
-      <c r="C88" s="49">
+      <c r="C88" s="60">
         <v>16</v>
       </c>
-      <c r="D88" s="49">
+      <c r="D88" s="60">
         <v>19</v>
       </c>
-      <c r="E88" s="49">
+      <c r="E88" s="60">
         <v>21</v>
       </c>
-      <c r="F88" s="58">
+      <c r="F88" s="61">
         <v>23</v>
       </c>
-      <c r="G88" s="49">
+      <c r="G88" s="60">
         <v>23</v>
       </c>
-      <c r="H88" s="55" t="s">
+      <c r="H88" s="62" t="s">
         <v>192</v>
       </c>
-      <c r="I88" s="46" t="s">
+      <c r="I88" s="68" t="s">
         <v>193</v>
       </c>
-      <c r="J88" s="49" t="s">
+      <c r="J88" s="60" t="s">
         <v>86</v>
       </c>
-      <c r="K88" s="49" t="s">
+      <c r="K88" s="60" t="s">
         <v>181</v>
       </c>
-      <c r="L88" s="46" t="s">
+      <c r="L88" s="68" t="s">
         <v>88</v>
       </c>
       <c r="M88" s="38" t="s">
         <v>194</v>
       </c>
-      <c r="N88" s="46" t="s">
+      <c r="N88" s="68" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="89" spans="2:19" ht="24">
-      <c r="B89" s="50"/>
-      <c r="C89" s="50"/>
-      <c r="D89" s="50"/>
-      <c r="E89" s="50"/>
-      <c r="F89" s="59"/>
-      <c r="G89" s="50"/>
-      <c r="H89" s="56"/>
-      <c r="I89" s="47"/>
-      <c r="J89" s="50"/>
-      <c r="K89" s="50"/>
-      <c r="L89" s="47"/>
+      <c r="B89" s="66"/>
+      <c r="C89" s="66"/>
+      <c r="D89" s="66"/>
+      <c r="E89" s="66"/>
+      <c r="F89" s="67"/>
+      <c r="G89" s="66"/>
+      <c r="H89" s="69"/>
+      <c r="I89" s="70"/>
+      <c r="J89" s="66"/>
+      <c r="K89" s="66"/>
+      <c r="L89" s="70"/>
       <c r="M89" s="14" t="s">
         <v>152</v>
       </c>
-      <c r="N89" s="47"/>
+      <c r="N89" s="70"/>
     </row>
     <row r="90" spans="2:19">
-      <c r="B90" s="50"/>
-      <c r="C90" s="50"/>
-      <c r="D90" s="50"/>
-      <c r="E90" s="50"/>
-      <c r="F90" s="59"/>
-      <c r="G90" s="50"/>
-      <c r="H90" s="56"/>
-      <c r="I90" s="47"/>
-      <c r="J90" s="50"/>
-      <c r="K90" s="50"/>
-      <c r="L90" s="47"/>
+      <c r="B90" s="66"/>
+      <c r="C90" s="66"/>
+      <c r="D90" s="66"/>
+      <c r="E90" s="66"/>
+      <c r="F90" s="67"/>
+      <c r="G90" s="66"/>
+      <c r="H90" s="69"/>
+      <c r="I90" s="70"/>
+      <c r="J90" s="66"/>
+      <c r="K90" s="66"/>
+      <c r="L90" s="70"/>
       <c r="M90" s="14" t="s">
         <v>195</v>
       </c>
-      <c r="N90" s="47"/>
+      <c r="N90" s="70"/>
     </row>
     <row r="91" spans="2:19">
-      <c r="B91" s="50"/>
-      <c r="C91" s="50"/>
-      <c r="D91" s="50"/>
-      <c r="E91" s="50"/>
-      <c r="F91" s="59"/>
-      <c r="G91" s="50"/>
-      <c r="H91" s="56"/>
-      <c r="I91" s="47"/>
-      <c r="J91" s="50"/>
-      <c r="K91" s="50"/>
-      <c r="L91" s="47"/>
+      <c r="B91" s="66"/>
+      <c r="C91" s="66"/>
+      <c r="D91" s="66"/>
+      <c r="E91" s="66"/>
+      <c r="F91" s="67"/>
+      <c r="G91" s="66"/>
+      <c r="H91" s="69"/>
+      <c r="I91" s="70"/>
+      <c r="J91" s="66"/>
+      <c r="K91" s="66"/>
+      <c r="L91" s="70"/>
       <c r="M91" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="N91" s="47"/>
+      <c r="N91" s="70"/>
     </row>
     <row r="92" spans="2:19" ht="24">
-      <c r="B92" s="50"/>
-      <c r="C92" s="50"/>
-      <c r="D92" s="50"/>
-      <c r="E92" s="50"/>
-      <c r="F92" s="59"/>
-      <c r="G92" s="50"/>
-      <c r="H92" s="56"/>
-      <c r="I92" s="47"/>
-      <c r="J92" s="50"/>
-      <c r="K92" s="50"/>
-      <c r="L92" s="47"/>
+      <c r="B92" s="66"/>
+      <c r="C92" s="66"/>
+      <c r="D92" s="66"/>
+      <c r="E92" s="66"/>
+      <c r="F92" s="67"/>
+      <c r="G92" s="66"/>
+      <c r="H92" s="69"/>
+      <c r="I92" s="70"/>
+      <c r="J92" s="66"/>
+      <c r="K92" s="66"/>
+      <c r="L92" s="70"/>
       <c r="M92" s="37" t="s">
         <v>107</v>
       </c>
-      <c r="N92" s="47"/>
+      <c r="N92" s="70"/>
     </row>
     <row r="93" spans="2:19" ht="24.75" thickBot="1">
       <c r="B93" s="51"/>
       <c r="C93" s="51"/>
       <c r="D93" s="51"/>
       <c r="E93" s="51"/>
-      <c r="F93" s="60"/>
+      <c r="F93" s="53"/>
       <c r="G93" s="51"/>
-      <c r="H93" s="57"/>
-      <c r="I93" s="48"/>
+      <c r="H93" s="59"/>
+      <c r="I93" s="57"/>
       <c r="J93" s="51"/>
       <c r="K93" s="51"/>
-      <c r="L93" s="48"/>
+      <c r="L93" s="57"/>
       <c r="M93" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="N93" s="48"/>
+      <c r="N93" s="57"/>
     </row>
     <row r="94" spans="2:19">
-      <c r="B94" s="49">
+      <c r="B94" s="60">
         <v>14</v>
       </c>
-      <c r="C94" s="49">
+      <c r="C94" s="60">
         <v>17</v>
       </c>
-      <c r="D94" s="49">
+      <c r="D94" s="60">
         <v>20</v>
       </c>
-      <c r="E94" s="49">
+      <c r="E94" s="60">
         <v>22</v>
       </c>
-      <c r="F94" s="58">
+      <c r="F94" s="61">
         <v>24</v>
       </c>
-      <c r="G94" s="49">
+      <c r="G94" s="60">
         <v>24</v>
       </c>
-      <c r="H94" s="55" t="s">
+      <c r="H94" s="62" t="s">
         <v>196</v>
       </c>
-      <c r="I94" s="46" t="s">
+      <c r="I94" s="68" t="s">
         <v>197</v>
       </c>
-      <c r="J94" s="49" t="s">
+      <c r="J94" s="60" t="s">
         <v>86</v>
       </c>
-      <c r="K94" s="49" t="s">
+      <c r="K94" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="L94" s="67">
+      <c r="L94" s="80">
         <v>-7</v>
       </c>
       <c r="M94" s="38" t="s">
         <v>198</v>
       </c>
-      <c r="N94" s="46" t="s">
+      <c r="N94" s="68" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="95" spans="2:19" ht="24">
-      <c r="B95" s="50"/>
-      <c r="C95" s="50"/>
-      <c r="D95" s="50"/>
-      <c r="E95" s="50"/>
-      <c r="F95" s="59"/>
-      <c r="G95" s="50"/>
-      <c r="H95" s="56"/>
-      <c r="I95" s="47"/>
-      <c r="J95" s="50"/>
-      <c r="K95" s="50"/>
-      <c r="L95" s="68"/>
+      <c r="B95" s="66"/>
+      <c r="C95" s="66"/>
+      <c r="D95" s="66"/>
+      <c r="E95" s="66"/>
+      <c r="F95" s="67"/>
+      <c r="G95" s="66"/>
+      <c r="H95" s="69"/>
+      <c r="I95" s="70"/>
+      <c r="J95" s="66"/>
+      <c r="K95" s="66"/>
+      <c r="L95" s="78"/>
       <c r="M95" s="23" t="s">
         <v>158</v>
       </c>
-      <c r="N95" s="47"/>
+      <c r="N95" s="70"/>
     </row>
     <row r="96" spans="2:19" ht="24">
-      <c r="B96" s="50"/>
-      <c r="C96" s="50"/>
-      <c r="D96" s="50"/>
-      <c r="E96" s="50"/>
-      <c r="F96" s="59"/>
-      <c r="G96" s="50"/>
-      <c r="H96" s="56"/>
-      <c r="I96" s="47"/>
-      <c r="J96" s="50"/>
-      <c r="K96" s="50"/>
-      <c r="L96" s="68"/>
+      <c r="B96" s="66"/>
+      <c r="C96" s="66"/>
+      <c r="D96" s="66"/>
+      <c r="E96" s="66"/>
+      <c r="F96" s="67"/>
+      <c r="G96" s="66"/>
+      <c r="H96" s="69"/>
+      <c r="I96" s="70"/>
+      <c r="J96" s="66"/>
+      <c r="K96" s="66"/>
+      <c r="L96" s="78"/>
       <c r="M96" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="N96" s="47"/>
+      <c r="N96" s="70"/>
     </row>
     <row r="97" spans="2:16" ht="24">
-      <c r="B97" s="50"/>
-      <c r="C97" s="50"/>
-      <c r="D97" s="50"/>
-      <c r="E97" s="50"/>
-      <c r="F97" s="59"/>
-      <c r="G97" s="50"/>
-      <c r="H97" s="56"/>
-      <c r="I97" s="47"/>
-      <c r="J97" s="50"/>
-      <c r="K97" s="50"/>
-      <c r="L97" s="68"/>
+      <c r="B97" s="66"/>
+      <c r="C97" s="66"/>
+      <c r="D97" s="66"/>
+      <c r="E97" s="66"/>
+      <c r="F97" s="67"/>
+      <c r="G97" s="66"/>
+      <c r="H97" s="69"/>
+      <c r="I97" s="70"/>
+      <c r="J97" s="66"/>
+      <c r="K97" s="66"/>
+      <c r="L97" s="78"/>
       <c r="M97" s="36" t="s">
         <v>125</v>
       </c>
-      <c r="N97" s="47"/>
+      <c r="N97" s="70"/>
     </row>
     <row r="98" spans="2:16">
-      <c r="B98" s="50"/>
-      <c r="C98" s="50"/>
-      <c r="D98" s="50"/>
-      <c r="E98" s="50"/>
-      <c r="F98" s="59"/>
-      <c r="G98" s="50"/>
-      <c r="H98" s="56"/>
-      <c r="I98" s="47"/>
-      <c r="J98" s="50"/>
-      <c r="K98" s="50"/>
-      <c r="L98" s="68"/>
+      <c r="B98" s="66"/>
+      <c r="C98" s="66"/>
+      <c r="D98" s="66"/>
+      <c r="E98" s="66"/>
+      <c r="F98" s="67"/>
+      <c r="G98" s="66"/>
+      <c r="H98" s="69"/>
+      <c r="I98" s="70"/>
+      <c r="J98" s="66"/>
+      <c r="K98" s="66"/>
+      <c r="L98" s="78"/>
       <c r="M98" s="14" t="s">
         <v>151</v>
       </c>
-      <c r="N98" s="47"/>
+      <c r="N98" s="70"/>
     </row>
     <row r="99" spans="2:16" ht="24">
-      <c r="B99" s="50"/>
-      <c r="C99" s="50"/>
-      <c r="D99" s="50"/>
-      <c r="E99" s="50"/>
-      <c r="F99" s="59"/>
-      <c r="G99" s="50"/>
-      <c r="H99" s="56"/>
-      <c r="I99" s="47"/>
-      <c r="J99" s="50"/>
-      <c r="K99" s="50"/>
-      <c r="L99" s="68"/>
+      <c r="B99" s="66"/>
+      <c r="C99" s="66"/>
+      <c r="D99" s="66"/>
+      <c r="E99" s="66"/>
+      <c r="F99" s="67"/>
+      <c r="G99" s="66"/>
+      <c r="H99" s="69"/>
+      <c r="I99" s="70"/>
+      <c r="J99" s="66"/>
+      <c r="K99" s="66"/>
+      <c r="L99" s="78"/>
       <c r="M99" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="N99" s="47"/>
+      <c r="N99" s="70"/>
     </row>
     <row r="100" spans="2:16" ht="24.75" thickBot="1">
       <c r="B100" s="51"/>
       <c r="C100" s="51"/>
       <c r="D100" s="51"/>
       <c r="E100" s="51"/>
-      <c r="F100" s="60"/>
+      <c r="F100" s="53"/>
       <c r="G100" s="51"/>
-      <c r="H100" s="57"/>
-      <c r="I100" s="48"/>
+      <c r="H100" s="59"/>
+      <c r="I100" s="57"/>
       <c r="J100" s="51"/>
       <c r="K100" s="51"/>
-      <c r="L100" s="69"/>
+      <c r="L100" s="79"/>
       <c r="M100" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="N100" s="48"/>
+      <c r="N100" s="57"/>
     </row>
     <row r="101" spans="2:16">
-      <c r="B101" s="46" t="s">
-        <v>88</v>
-      </c>
-      <c r="C101" s="46" t="s">
-        <v>88</v>
-      </c>
-      <c r="D101" s="46" t="s">
-        <v>88</v>
-      </c>
-      <c r="E101" s="49">
+      <c r="B101" s="68" t="s">
+        <v>88</v>
+      </c>
+      <c r="C101" s="68" t="s">
+        <v>88</v>
+      </c>
+      <c r="D101" s="68" t="s">
+        <v>88</v>
+      </c>
+      <c r="E101" s="60">
         <v>23</v>
       </c>
-      <c r="F101" s="58">
+      <c r="F101" s="61">
         <v>25</v>
       </c>
-      <c r="G101" s="49">
+      <c r="G101" s="60">
         <v>25</v>
       </c>
-      <c r="H101" s="46" t="s">
-        <v>88</v>
-      </c>
-      <c r="I101" s="46" t="s">
+      <c r="H101" s="68" t="s">
+        <v>88</v>
+      </c>
+      <c r="I101" s="68" t="s">
         <v>199</v>
       </c>
-      <c r="J101" s="49" t="s">
+      <c r="J101" s="60" t="s">
         <v>86</v>
       </c>
-      <c r="K101" s="49" t="s">
+      <c r="K101" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="L101" s="46" t="s">
+      <c r="L101" s="68" t="s">
         <v>88</v>
       </c>
       <c r="M101" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="N101" s="46" t="s">
+      <c r="N101" s="68" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="102" spans="2:16">
-      <c r="B102" s="47"/>
-      <c r="C102" s="47"/>
-      <c r="D102" s="47"/>
-      <c r="E102" s="50"/>
-      <c r="F102" s="59"/>
-      <c r="G102" s="50"/>
-      <c r="H102" s="47"/>
-      <c r="I102" s="47"/>
-      <c r="J102" s="50"/>
-      <c r="K102" s="50"/>
-      <c r="L102" s="47"/>
+      <c r="B102" s="70"/>
+      <c r="C102" s="70"/>
+      <c r="D102" s="70"/>
+      <c r="E102" s="66"/>
+      <c r="F102" s="67"/>
+      <c r="G102" s="66"/>
+      <c r="H102" s="70"/>
+      <c r="I102" s="70"/>
+      <c r="J102" s="66"/>
+      <c r="K102" s="66"/>
+      <c r="L102" s="70"/>
       <c r="M102" s="14" t="s">
         <v>142</v>
       </c>
-      <c r="N102" s="47"/>
+      <c r="N102" s="70"/>
     </row>
     <row r="103" spans="2:16" ht="24">
-      <c r="B103" s="47"/>
-      <c r="C103" s="47"/>
-      <c r="D103" s="47"/>
-      <c r="E103" s="50"/>
-      <c r="F103" s="59"/>
-      <c r="G103" s="50"/>
-      <c r="H103" s="47"/>
-      <c r="I103" s="47"/>
-      <c r="J103" s="50"/>
-      <c r="K103" s="50"/>
-      <c r="L103" s="47"/>
+      <c r="B103" s="70"/>
+      <c r="C103" s="70"/>
+      <c r="D103" s="70"/>
+      <c r="E103" s="66"/>
+      <c r="F103" s="67"/>
+      <c r="G103" s="66"/>
+      <c r="H103" s="70"/>
+      <c r="I103" s="70"/>
+      <c r="J103" s="66"/>
+      <c r="K103" s="66"/>
+      <c r="L103" s="70"/>
       <c r="M103" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="N103" s="47"/>
+      <c r="N103" s="70"/>
     </row>
     <row r="104" spans="2:16" ht="24">
-      <c r="B104" s="47"/>
-      <c r="C104" s="47"/>
-      <c r="D104" s="47"/>
-      <c r="E104" s="50"/>
-      <c r="F104" s="59"/>
-      <c r="G104" s="50"/>
-      <c r="H104" s="47"/>
-      <c r="I104" s="47"/>
-      <c r="J104" s="50"/>
-      <c r="K104" s="50"/>
-      <c r="L104" s="47"/>
+      <c r="B104" s="70"/>
+      <c r="C104" s="70"/>
+      <c r="D104" s="70"/>
+      <c r="E104" s="66"/>
+      <c r="F104" s="67"/>
+      <c r="G104" s="66"/>
+      <c r="H104" s="70"/>
+      <c r="I104" s="70"/>
+      <c r="J104" s="66"/>
+      <c r="K104" s="66"/>
+      <c r="L104" s="70"/>
       <c r="M104" s="29" t="s">
         <v>103</v>
       </c>
-      <c r="N104" s="47"/>
+      <c r="N104" s="70"/>
     </row>
     <row r="105" spans="2:16" ht="15" thickBot="1">
-      <c r="B105" s="48"/>
-      <c r="C105" s="48"/>
-      <c r="D105" s="48"/>
+      <c r="B105" s="57"/>
+      <c r="C105" s="57"/>
+      <c r="D105" s="57"/>
       <c r="E105" s="51"/>
-      <c r="F105" s="60"/>
+      <c r="F105" s="53"/>
       <c r="G105" s="51"/>
-      <c r="H105" s="48"/>
-      <c r="I105" s="48"/>
+      <c r="H105" s="57"/>
+      <c r="I105" s="57"/>
       <c r="J105" s="51"/>
       <c r="K105" s="51"/>
-      <c r="L105" s="48"/>
+      <c r="L105" s="57"/>
       <c r="M105" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="N105" s="48"/>
+      <c r="N105" s="57"/>
     </row>
     <row r="106" spans="2:16">
-      <c r="B106" s="46" t="s">
-        <v>88</v>
-      </c>
-      <c r="C106" s="46" t="s">
-        <v>88</v>
-      </c>
-      <c r="D106" s="46" t="s">
-        <v>88</v>
-      </c>
-      <c r="E106" s="49">
+      <c r="B106" s="68" t="s">
+        <v>88</v>
+      </c>
+      <c r="C106" s="68" t="s">
+        <v>88</v>
+      </c>
+      <c r="D106" s="68" t="s">
+        <v>88</v>
+      </c>
+      <c r="E106" s="60">
         <v>24</v>
       </c>
-      <c r="F106" s="58">
+      <c r="F106" s="61">
         <v>26</v>
       </c>
-      <c r="G106" s="49">
+      <c r="G106" s="60">
         <v>26</v>
       </c>
-      <c r="H106" s="55" t="s">
+      <c r="H106" s="62" t="s">
         <v>200</v>
       </c>
-      <c r="I106" s="70" t="s">
+      <c r="I106" s="74" t="s">
         <v>201</v>
       </c>
-      <c r="J106" s="49" t="s">
+      <c r="J106" s="60" t="s">
         <v>86</v>
       </c>
-      <c r="K106" s="49" t="s">
+      <c r="K106" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="L106" s="46" t="s">
+      <c r="L106" s="68" t="s">
         <v>88</v>
       </c>
       <c r="M106" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="N106" s="46" t="s">
+      <c r="N106" s="68" t="s">
         <v>203</v>
       </c>
       <c r="P106" t="s">
@@ -6891,38 +6915,38 @@
       </c>
     </row>
     <row r="107" spans="2:16">
-      <c r="B107" s="47"/>
-      <c r="C107" s="47"/>
-      <c r="D107" s="47"/>
-      <c r="E107" s="50"/>
-      <c r="F107" s="59"/>
-      <c r="G107" s="50"/>
-      <c r="H107" s="56"/>
-      <c r="I107" s="65"/>
-      <c r="J107" s="50"/>
-      <c r="K107" s="50"/>
-      <c r="L107" s="47"/>
+      <c r="B107" s="70"/>
+      <c r="C107" s="70"/>
+      <c r="D107" s="70"/>
+      <c r="E107" s="66"/>
+      <c r="F107" s="67"/>
+      <c r="G107" s="66"/>
+      <c r="H107" s="69"/>
+      <c r="I107" s="75"/>
+      <c r="J107" s="66"/>
+      <c r="K107" s="66"/>
+      <c r="L107" s="70"/>
       <c r="M107" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="N107" s="47"/>
+      <c r="N107" s="70"/>
     </row>
     <row r="108" spans="2:16" ht="15" thickBot="1">
-      <c r="B108" s="48"/>
-      <c r="C108" s="48"/>
-      <c r="D108" s="48"/>
+      <c r="B108" s="57"/>
+      <c r="C108" s="57"/>
+      <c r="D108" s="57"/>
       <c r="E108" s="51"/>
-      <c r="F108" s="60"/>
+      <c r="F108" s="53"/>
       <c r="G108" s="51"/>
-      <c r="H108" s="57"/>
-      <c r="I108" s="66"/>
+      <c r="H108" s="59"/>
+      <c r="I108" s="76"/>
       <c r="J108" s="51"/>
       <c r="K108" s="51"/>
-      <c r="L108" s="48"/>
+      <c r="L108" s="57"/>
       <c r="M108" s="19" t="s">
         <v>202</v>
       </c>
-      <c r="N108" s="48"/>
+      <c r="N108" s="57"/>
     </row>
     <row r="109" spans="2:16" ht="24.75" thickBot="1">
       <c r="B109" s="24" t="s">
@@ -6969,43 +6993,43 @@
       </c>
     </row>
     <row r="110" spans="2:16" ht="15" thickTop="1">
-      <c r="B110" s="61" t="s">
-        <v>88</v>
-      </c>
-      <c r="C110" s="61" t="s">
-        <v>88</v>
-      </c>
-      <c r="D110" s="61" t="s">
-        <v>88</v>
-      </c>
-      <c r="E110" s="62">
+      <c r="B110" s="56" t="s">
+        <v>88</v>
+      </c>
+      <c r="C110" s="56" t="s">
+        <v>88</v>
+      </c>
+      <c r="D110" s="56" t="s">
+        <v>88</v>
+      </c>
+      <c r="E110" s="50">
         <v>26</v>
       </c>
-      <c r="F110" s="63">
+      <c r="F110" s="52">
         <v>28</v>
       </c>
-      <c r="G110" s="62">
+      <c r="G110" s="50">
         <v>28</v>
       </c>
-      <c r="H110" s="61" t="s">
-        <v>88</v>
-      </c>
-      <c r="I110" s="64" t="s">
+      <c r="H110" s="56" t="s">
+        <v>88</v>
+      </c>
+      <c r="I110" s="81" t="s">
         <v>207</v>
       </c>
-      <c r="J110" s="62" t="s">
+      <c r="J110" s="50" t="s">
         <v>86</v>
       </c>
-      <c r="K110" s="62" t="s">
+      <c r="K110" s="50" t="s">
         <v>87</v>
       </c>
-      <c r="L110" s="61" t="s">
+      <c r="L110" s="56" t="s">
         <v>88</v>
       </c>
       <c r="M110" s="14" t="s">
         <v>157</v>
       </c>
-      <c r="N110" s="61" t="s">
+      <c r="N110" s="56" t="s">
         <v>206</v>
       </c>
       <c r="P110" t="s">
@@ -7013,222 +7037,222 @@
       </c>
     </row>
     <row r="111" spans="2:16" ht="24">
-      <c r="B111" s="47"/>
-      <c r="C111" s="47"/>
-      <c r="D111" s="47"/>
-      <c r="E111" s="50"/>
-      <c r="F111" s="59"/>
-      <c r="G111" s="50"/>
-      <c r="H111" s="47"/>
-      <c r="I111" s="65"/>
-      <c r="J111" s="50"/>
-      <c r="K111" s="50"/>
-      <c r="L111" s="47"/>
+      <c r="B111" s="70"/>
+      <c r="C111" s="70"/>
+      <c r="D111" s="70"/>
+      <c r="E111" s="66"/>
+      <c r="F111" s="67"/>
+      <c r="G111" s="66"/>
+      <c r="H111" s="70"/>
+      <c r="I111" s="75"/>
+      <c r="J111" s="66"/>
+      <c r="K111" s="66"/>
+      <c r="L111" s="70"/>
       <c r="M111" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="N111" s="47"/>
+      <c r="N111" s="70"/>
     </row>
     <row r="112" spans="2:16" ht="24">
-      <c r="B112" s="47"/>
-      <c r="C112" s="47"/>
-      <c r="D112" s="47"/>
-      <c r="E112" s="50"/>
-      <c r="F112" s="59"/>
-      <c r="G112" s="50"/>
-      <c r="H112" s="47"/>
-      <c r="I112" s="65"/>
-      <c r="J112" s="50"/>
-      <c r="K112" s="50"/>
-      <c r="L112" s="47"/>
+      <c r="B112" s="70"/>
+      <c r="C112" s="70"/>
+      <c r="D112" s="70"/>
+      <c r="E112" s="66"/>
+      <c r="F112" s="67"/>
+      <c r="G112" s="66"/>
+      <c r="H112" s="70"/>
+      <c r="I112" s="75"/>
+      <c r="J112" s="66"/>
+      <c r="K112" s="66"/>
+      <c r="L112" s="70"/>
       <c r="M112" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="N112" s="47"/>
+      <c r="N112" s="70"/>
     </row>
     <row r="113" spans="2:14" ht="15" thickBot="1">
-      <c r="B113" s="48"/>
-      <c r="C113" s="48"/>
-      <c r="D113" s="48"/>
+      <c r="B113" s="57"/>
+      <c r="C113" s="57"/>
+      <c r="D113" s="57"/>
       <c r="E113" s="51"/>
-      <c r="F113" s="60"/>
+      <c r="F113" s="53"/>
       <c r="G113" s="51"/>
-      <c r="H113" s="48"/>
-      <c r="I113" s="66"/>
+      <c r="H113" s="57"/>
+      <c r="I113" s="76"/>
       <c r="J113" s="51"/>
       <c r="K113" s="51"/>
-      <c r="L113" s="48"/>
+      <c r="L113" s="57"/>
       <c r="M113" s="19" t="s">
         <v>208</v>
       </c>
-      <c r="N113" s="48"/>
+      <c r="N113" s="57"/>
     </row>
     <row r="114" spans="2:14" ht="36">
-      <c r="B114" s="46" t="s">
-        <v>88</v>
-      </c>
-      <c r="C114" s="49">
+      <c r="B114" s="68" t="s">
+        <v>88</v>
+      </c>
+      <c r="C114" s="60">
         <v>18</v>
       </c>
-      <c r="D114" s="46" t="s">
-        <v>88</v>
-      </c>
-      <c r="E114" s="49">
+      <c r="D114" s="68" t="s">
+        <v>88</v>
+      </c>
+      <c r="E114" s="60">
         <v>27</v>
       </c>
-      <c r="F114" s="58">
+      <c r="F114" s="61">
         <v>29</v>
       </c>
-      <c r="G114" s="49">
+      <c r="G114" s="60">
         <v>29</v>
       </c>
-      <c r="H114" s="55" t="s">
+      <c r="H114" s="62" t="s">
         <v>209</v>
       </c>
-      <c r="I114" s="46" t="s">
+      <c r="I114" s="68" t="s">
         <v>210</v>
       </c>
-      <c r="J114" s="49" t="s">
+      <c r="J114" s="60" t="s">
         <v>86</v>
       </c>
-      <c r="K114" s="49" t="s">
+      <c r="K114" s="60" t="s">
         <v>181</v>
       </c>
-      <c r="L114" s="46" t="s">
+      <c r="L114" s="68" t="s">
         <v>88</v>
       </c>
       <c r="M114" s="29" t="s">
         <v>211</v>
       </c>
-      <c r="N114" s="46" t="s">
+      <c r="N114" s="68" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="115" spans="2:14" ht="24">
-      <c r="B115" s="47"/>
-      <c r="C115" s="50"/>
-      <c r="D115" s="47"/>
-      <c r="E115" s="50"/>
-      <c r="F115" s="59"/>
-      <c r="G115" s="50"/>
-      <c r="H115" s="56"/>
-      <c r="I115" s="47"/>
-      <c r="J115" s="50"/>
-      <c r="K115" s="50"/>
-      <c r="L115" s="47"/>
+      <c r="B115" s="70"/>
+      <c r="C115" s="66"/>
+      <c r="D115" s="70"/>
+      <c r="E115" s="66"/>
+      <c r="F115" s="67"/>
+      <c r="G115" s="66"/>
+      <c r="H115" s="69"/>
+      <c r="I115" s="70"/>
+      <c r="J115" s="66"/>
+      <c r="K115" s="66"/>
+      <c r="L115" s="70"/>
       <c r="M115" s="14" t="s">
         <v>152</v>
       </c>
-      <c r="N115" s="47"/>
+      <c r="N115" s="70"/>
     </row>
     <row r="116" spans="2:14">
-      <c r="B116" s="47"/>
-      <c r="C116" s="50"/>
-      <c r="D116" s="47"/>
-      <c r="E116" s="50"/>
-      <c r="F116" s="59"/>
-      <c r="G116" s="50"/>
-      <c r="H116" s="56"/>
-      <c r="I116" s="47"/>
-      <c r="J116" s="50"/>
-      <c r="K116" s="50"/>
-      <c r="L116" s="47"/>
+      <c r="B116" s="70"/>
+      <c r="C116" s="66"/>
+      <c r="D116" s="70"/>
+      <c r="E116" s="66"/>
+      <c r="F116" s="67"/>
+      <c r="G116" s="66"/>
+      <c r="H116" s="69"/>
+      <c r="I116" s="70"/>
+      <c r="J116" s="66"/>
+      <c r="K116" s="66"/>
+      <c r="L116" s="70"/>
       <c r="M116" s="14" t="s">
         <v>188</v>
       </c>
-      <c r="N116" s="47"/>
+      <c r="N116" s="70"/>
     </row>
     <row r="117" spans="2:14" ht="24.75" thickBot="1">
-      <c r="B117" s="48"/>
+      <c r="B117" s="57"/>
       <c r="C117" s="51"/>
-      <c r="D117" s="48"/>
+      <c r="D117" s="57"/>
       <c r="E117" s="51"/>
-      <c r="F117" s="60"/>
+      <c r="F117" s="53"/>
       <c r="G117" s="51"/>
-      <c r="H117" s="57"/>
-      <c r="I117" s="48"/>
+      <c r="H117" s="59"/>
+      <c r="I117" s="57"/>
       <c r="J117" s="51"/>
       <c r="K117" s="51"/>
-      <c r="L117" s="48"/>
+      <c r="L117" s="57"/>
       <c r="M117" s="34" t="s">
         <v>121</v>
       </c>
-      <c r="N117" s="48"/>
+      <c r="N117" s="57"/>
     </row>
     <row r="118" spans="2:14" ht="36">
-      <c r="B118" s="46" t="s">
-        <v>88</v>
-      </c>
-      <c r="C118" s="49">
+      <c r="B118" s="68" t="s">
+        <v>88</v>
+      </c>
+      <c r="C118" s="60">
         <v>19</v>
       </c>
-      <c r="D118" s="46" t="s">
-        <v>88</v>
-      </c>
-      <c r="E118" s="49">
+      <c r="D118" s="68" t="s">
+        <v>88</v>
+      </c>
+      <c r="E118" s="60">
         <v>28</v>
       </c>
-      <c r="F118" s="58">
+      <c r="F118" s="61">
         <v>30</v>
       </c>
-      <c r="G118" s="49">
+      <c r="G118" s="60">
         <v>30</v>
       </c>
-      <c r="H118" s="55" t="s">
+      <c r="H118" s="62" t="s">
         <v>212</v>
       </c>
-      <c r="I118" s="46" t="s">
+      <c r="I118" s="68" t="s">
         <v>213</v>
       </c>
-      <c r="J118" s="49" t="s">
+      <c r="J118" s="60" t="s">
         <v>86</v>
       </c>
-      <c r="K118" s="49" t="s">
+      <c r="K118" s="60" t="s">
         <v>181</v>
       </c>
-      <c r="L118" s="46" t="s">
+      <c r="L118" s="68" t="s">
         <v>88</v>
       </c>
       <c r="M118" s="29" t="s">
         <v>214</v>
       </c>
-      <c r="N118" s="46" t="s">
+      <c r="N118" s="68" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="119" spans="2:14" ht="36">
-      <c r="B119" s="47"/>
-      <c r="C119" s="50"/>
-      <c r="D119" s="47"/>
-      <c r="E119" s="50"/>
-      <c r="F119" s="59"/>
-      <c r="G119" s="50"/>
-      <c r="H119" s="56"/>
-      <c r="I119" s="47"/>
-      <c r="J119" s="50"/>
-      <c r="K119" s="50"/>
-      <c r="L119" s="47"/>
+      <c r="B119" s="70"/>
+      <c r="C119" s="66"/>
+      <c r="D119" s="70"/>
+      <c r="E119" s="66"/>
+      <c r="F119" s="67"/>
+      <c r="G119" s="66"/>
+      <c r="H119" s="69"/>
+      <c r="I119" s="70"/>
+      <c r="J119" s="66"/>
+      <c r="K119" s="66"/>
+      <c r="L119" s="70"/>
       <c r="M119" s="14" t="s">
         <v>215</v>
       </c>
-      <c r="N119" s="47"/>
+      <c r="N119" s="70"/>
     </row>
     <row r="120" spans="2:14" ht="24.75" thickBot="1">
-      <c r="B120" s="48"/>
+      <c r="B120" s="57"/>
       <c r="C120" s="51"/>
-      <c r="D120" s="48"/>
+      <c r="D120" s="57"/>
       <c r="E120" s="51"/>
-      <c r="F120" s="60"/>
+      <c r="F120" s="53"/>
       <c r="G120" s="51"/>
-      <c r="H120" s="57"/>
-      <c r="I120" s="48"/>
+      <c r="H120" s="59"/>
+      <c r="I120" s="57"/>
       <c r="J120" s="51"/>
       <c r="K120" s="51"/>
-      <c r="L120" s="48"/>
+      <c r="L120" s="57"/>
       <c r="M120" s="34" t="s">
         <v>136</v>
       </c>
-      <c r="N120" s="48"/>
+      <c r="N120" s="57"/>
     </row>
     <row r="121" spans="2:14" ht="48.75" thickBot="1">
       <c r="B121" s="17">
@@ -7272,96 +7296,96 @@
       </c>
     </row>
     <row r="122" spans="2:14" ht="24">
-      <c r="B122" s="46" t="s">
-        <v>88</v>
-      </c>
-      <c r="C122" s="46" t="s">
-        <v>88</v>
-      </c>
-      <c r="D122" s="46" t="s">
-        <v>88</v>
-      </c>
-      <c r="E122" s="46" t="s">
-        <v>88</v>
-      </c>
-      <c r="F122" s="52" t="s">
-        <v>88</v>
-      </c>
-      <c r="G122" s="49">
+      <c r="B122" s="68" t="s">
+        <v>88</v>
+      </c>
+      <c r="C122" s="68" t="s">
+        <v>88</v>
+      </c>
+      <c r="D122" s="68" t="s">
+        <v>88</v>
+      </c>
+      <c r="E122" s="68" t="s">
+        <v>88</v>
+      </c>
+      <c r="F122" s="82" t="s">
+        <v>88</v>
+      </c>
+      <c r="G122" s="60">
         <v>32</v>
       </c>
-      <c r="H122" s="46" t="s">
-        <v>88</v>
-      </c>
-      <c r="I122" s="46" t="s">
+      <c r="H122" s="68" t="s">
+        <v>88</v>
+      </c>
+      <c r="I122" s="68" t="s">
         <v>222</v>
       </c>
-      <c r="J122" s="49" t="s">
+      <c r="J122" s="60" t="s">
         <v>86</v>
       </c>
-      <c r="K122" s="49" t="s">
+      <c r="K122" s="60" t="s">
         <v>181</v>
       </c>
-      <c r="L122" s="46" t="s">
+      <c r="L122" s="68" t="s">
         <v>88</v>
       </c>
       <c r="M122" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="N122" s="46" t="s">
+      <c r="N122" s="68" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="123" spans="2:14" ht="24">
-      <c r="B123" s="47"/>
-      <c r="C123" s="47"/>
-      <c r="D123" s="47"/>
-      <c r="E123" s="47"/>
-      <c r="F123" s="53"/>
-      <c r="G123" s="50"/>
-      <c r="H123" s="47"/>
-      <c r="I123" s="47"/>
-      <c r="J123" s="50"/>
-      <c r="K123" s="50"/>
-      <c r="L123" s="47"/>
+      <c r="B123" s="70"/>
+      <c r="C123" s="70"/>
+      <c r="D123" s="70"/>
+      <c r="E123" s="70"/>
+      <c r="F123" s="83"/>
+      <c r="G123" s="66"/>
+      <c r="H123" s="70"/>
+      <c r="I123" s="70"/>
+      <c r="J123" s="66"/>
+      <c r="K123" s="66"/>
+      <c r="L123" s="70"/>
       <c r="M123" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="N123" s="47"/>
+      <c r="N123" s="70"/>
     </row>
     <row r="124" spans="2:14">
-      <c r="B124" s="47"/>
-      <c r="C124" s="47"/>
-      <c r="D124" s="47"/>
-      <c r="E124" s="47"/>
-      <c r="F124" s="53"/>
-      <c r="G124" s="50"/>
-      <c r="H124" s="47"/>
-      <c r="I124" s="47"/>
-      <c r="J124" s="50"/>
-      <c r="K124" s="50"/>
-      <c r="L124" s="47"/>
+      <c r="B124" s="70"/>
+      <c r="C124" s="70"/>
+      <c r="D124" s="70"/>
+      <c r="E124" s="70"/>
+      <c r="F124" s="83"/>
+      <c r="G124" s="66"/>
+      <c r="H124" s="70"/>
+      <c r="I124" s="70"/>
+      <c r="J124" s="66"/>
+      <c r="K124" s="66"/>
+      <c r="L124" s="70"/>
       <c r="M124" s="14" t="s">
         <v>223</v>
       </c>
-      <c r="N124" s="47"/>
+      <c r="N124" s="70"/>
     </row>
     <row r="125" spans="2:14" ht="15" thickBot="1">
-      <c r="B125" s="48"/>
-      <c r="C125" s="48"/>
-      <c r="D125" s="48"/>
-      <c r="E125" s="48"/>
-      <c r="F125" s="54"/>
+      <c r="B125" s="57"/>
+      <c r="C125" s="57"/>
+      <c r="D125" s="57"/>
+      <c r="E125" s="57"/>
+      <c r="F125" s="84"/>
       <c r="G125" s="51"/>
-      <c r="H125" s="48"/>
-      <c r="I125" s="48"/>
+      <c r="H125" s="57"/>
+      <c r="I125" s="57"/>
       <c r="J125" s="51"/>
       <c r="K125" s="51"/>
-      <c r="L125" s="48"/>
+      <c r="L125" s="57"/>
       <c r="M125" s="19" t="s">
         <v>224</v>
       </c>
-      <c r="N125" s="48"/>
+      <c r="N125" s="57"/>
     </row>
     <row r="126" spans="2:14" ht="15" thickBot="1">
       <c r="B126" s="24" t="s">
@@ -7447,32 +7471,254 @@
     </row>
   </sheetData>
   <mergeCells count="298">
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="N5:N6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="H122:H125"/>
+    <mergeCell ref="I122:I125"/>
+    <mergeCell ref="J122:J125"/>
+    <mergeCell ref="K122:K125"/>
+    <mergeCell ref="L122:L125"/>
+    <mergeCell ref="N122:N125"/>
+    <mergeCell ref="B122:B125"/>
+    <mergeCell ref="C122:C125"/>
+    <mergeCell ref="D122:D125"/>
+    <mergeCell ref="E122:E125"/>
+    <mergeCell ref="F122:F125"/>
+    <mergeCell ref="G122:G125"/>
+    <mergeCell ref="H118:H120"/>
+    <mergeCell ref="I118:I120"/>
+    <mergeCell ref="J118:J120"/>
+    <mergeCell ref="K118:K120"/>
+    <mergeCell ref="L118:L120"/>
+    <mergeCell ref="N118:N120"/>
+    <mergeCell ref="B118:B120"/>
+    <mergeCell ref="C118:C120"/>
+    <mergeCell ref="D118:D120"/>
+    <mergeCell ref="E118:E120"/>
+    <mergeCell ref="F118:F120"/>
+    <mergeCell ref="G118:G120"/>
+    <mergeCell ref="K114:K117"/>
+    <mergeCell ref="L114:L117"/>
+    <mergeCell ref="N114:N117"/>
+    <mergeCell ref="B114:B117"/>
+    <mergeCell ref="C114:C117"/>
+    <mergeCell ref="D114:D117"/>
+    <mergeCell ref="E114:E117"/>
+    <mergeCell ref="F114:F117"/>
+    <mergeCell ref="G114:G117"/>
+    <mergeCell ref="B110:B113"/>
+    <mergeCell ref="C110:C113"/>
+    <mergeCell ref="D110:D113"/>
+    <mergeCell ref="E110:E113"/>
+    <mergeCell ref="F110:F113"/>
+    <mergeCell ref="G110:G113"/>
+    <mergeCell ref="H114:H117"/>
+    <mergeCell ref="I114:I117"/>
+    <mergeCell ref="J114:J117"/>
+    <mergeCell ref="K101:K105"/>
+    <mergeCell ref="L101:L105"/>
+    <mergeCell ref="N101:N105"/>
+    <mergeCell ref="H110:H113"/>
+    <mergeCell ref="I110:I113"/>
+    <mergeCell ref="J110:J113"/>
+    <mergeCell ref="K110:K113"/>
+    <mergeCell ref="L110:L113"/>
+    <mergeCell ref="N110:N113"/>
+    <mergeCell ref="B106:B108"/>
+    <mergeCell ref="C106:C108"/>
+    <mergeCell ref="D106:D108"/>
+    <mergeCell ref="E106:E108"/>
+    <mergeCell ref="F106:F108"/>
+    <mergeCell ref="K94:K100"/>
+    <mergeCell ref="L94:L100"/>
+    <mergeCell ref="N94:N100"/>
+    <mergeCell ref="B101:B105"/>
+    <mergeCell ref="C101:C105"/>
+    <mergeCell ref="D101:D105"/>
+    <mergeCell ref="E101:E105"/>
+    <mergeCell ref="F101:F105"/>
+    <mergeCell ref="G101:G105"/>
+    <mergeCell ref="H101:H105"/>
+    <mergeCell ref="N106:N108"/>
+    <mergeCell ref="G106:G108"/>
+    <mergeCell ref="H106:H108"/>
+    <mergeCell ref="I106:I108"/>
+    <mergeCell ref="J106:J108"/>
+    <mergeCell ref="K106:K108"/>
+    <mergeCell ref="L106:L108"/>
+    <mergeCell ref="I101:I105"/>
+    <mergeCell ref="J101:J105"/>
+    <mergeCell ref="B94:B100"/>
+    <mergeCell ref="C94:C100"/>
+    <mergeCell ref="D94:D100"/>
+    <mergeCell ref="E94:E100"/>
+    <mergeCell ref="F94:F100"/>
+    <mergeCell ref="G94:G100"/>
+    <mergeCell ref="H94:H100"/>
+    <mergeCell ref="I94:I100"/>
+    <mergeCell ref="J94:J100"/>
+    <mergeCell ref="K84:K87"/>
+    <mergeCell ref="L84:L87"/>
+    <mergeCell ref="N84:N87"/>
+    <mergeCell ref="B88:B93"/>
+    <mergeCell ref="C88:C93"/>
+    <mergeCell ref="D88:D93"/>
+    <mergeCell ref="E88:E93"/>
+    <mergeCell ref="F88:F93"/>
+    <mergeCell ref="N88:N93"/>
+    <mergeCell ref="G88:G93"/>
+    <mergeCell ref="H88:H93"/>
+    <mergeCell ref="I88:I93"/>
+    <mergeCell ref="J88:J93"/>
+    <mergeCell ref="K88:K93"/>
+    <mergeCell ref="L88:L93"/>
+    <mergeCell ref="B84:B87"/>
+    <mergeCell ref="C84:C87"/>
+    <mergeCell ref="D84:D87"/>
+    <mergeCell ref="E84:E87"/>
+    <mergeCell ref="F84:F87"/>
+    <mergeCell ref="G84:G87"/>
+    <mergeCell ref="H84:H87"/>
+    <mergeCell ref="I84:I87"/>
+    <mergeCell ref="J84:J87"/>
+    <mergeCell ref="N75:N79"/>
+    <mergeCell ref="B80:B83"/>
+    <mergeCell ref="C80:C83"/>
+    <mergeCell ref="D80:D83"/>
+    <mergeCell ref="E80:E83"/>
+    <mergeCell ref="F80:F83"/>
+    <mergeCell ref="G80:G83"/>
+    <mergeCell ref="H80:H83"/>
+    <mergeCell ref="I80:I83"/>
+    <mergeCell ref="J80:J83"/>
+    <mergeCell ref="G75:G79"/>
+    <mergeCell ref="H75:H79"/>
+    <mergeCell ref="I75:I79"/>
+    <mergeCell ref="J75:J79"/>
+    <mergeCell ref="K75:K79"/>
+    <mergeCell ref="L75:L79"/>
+    <mergeCell ref="B75:B79"/>
+    <mergeCell ref="C75:C79"/>
+    <mergeCell ref="D75:D79"/>
+    <mergeCell ref="E75:E79"/>
+    <mergeCell ref="F75:F79"/>
+    <mergeCell ref="K80:K83"/>
+    <mergeCell ref="L80:L83"/>
+    <mergeCell ref="N80:N83"/>
+    <mergeCell ref="H71:H74"/>
+    <mergeCell ref="I71:I74"/>
+    <mergeCell ref="J71:J74"/>
+    <mergeCell ref="K71:K74"/>
+    <mergeCell ref="L71:L74"/>
+    <mergeCell ref="N71:N74"/>
+    <mergeCell ref="B71:B74"/>
+    <mergeCell ref="C71:C74"/>
+    <mergeCell ref="D71:D74"/>
+    <mergeCell ref="E71:E74"/>
+    <mergeCell ref="F71:F74"/>
+    <mergeCell ref="G71:G74"/>
+    <mergeCell ref="H67:H70"/>
+    <mergeCell ref="I67:I70"/>
+    <mergeCell ref="J67:J70"/>
+    <mergeCell ref="K67:K70"/>
+    <mergeCell ref="L67:L70"/>
+    <mergeCell ref="N67:N70"/>
+    <mergeCell ref="B67:B70"/>
+    <mergeCell ref="C67:C70"/>
+    <mergeCell ref="D67:D70"/>
+    <mergeCell ref="E67:E70"/>
+    <mergeCell ref="F67:F70"/>
+    <mergeCell ref="G67:G70"/>
+    <mergeCell ref="G59:G63"/>
+    <mergeCell ref="H59:H63"/>
+    <mergeCell ref="I59:I63"/>
+    <mergeCell ref="J59:J63"/>
+    <mergeCell ref="K59:K63"/>
+    <mergeCell ref="L59:L63"/>
+    <mergeCell ref="H54:H58"/>
+    <mergeCell ref="I54:I58"/>
+    <mergeCell ref="J54:J58"/>
+    <mergeCell ref="K54:K58"/>
+    <mergeCell ref="L54:L58"/>
+    <mergeCell ref="G54:G58"/>
+    <mergeCell ref="B59:B63"/>
+    <mergeCell ref="C59:C63"/>
+    <mergeCell ref="D59:D63"/>
+    <mergeCell ref="E59:E63"/>
+    <mergeCell ref="F59:F63"/>
+    <mergeCell ref="B54:B58"/>
+    <mergeCell ref="C54:C58"/>
+    <mergeCell ref="D54:D58"/>
+    <mergeCell ref="E54:E58"/>
+    <mergeCell ref="F54:F58"/>
+    <mergeCell ref="H48:H53"/>
+    <mergeCell ref="I48:I53"/>
+    <mergeCell ref="J48:J53"/>
+    <mergeCell ref="K48:K53"/>
+    <mergeCell ref="L48:L53"/>
+    <mergeCell ref="J43:J47"/>
+    <mergeCell ref="K43:K47"/>
+    <mergeCell ref="L43:L47"/>
+    <mergeCell ref="N43:N47"/>
+    <mergeCell ref="N48:N49"/>
+    <mergeCell ref="B48:B53"/>
+    <mergeCell ref="C48:C53"/>
+    <mergeCell ref="D48:D53"/>
+    <mergeCell ref="E48:E53"/>
+    <mergeCell ref="F48:F53"/>
+    <mergeCell ref="G48:G53"/>
+    <mergeCell ref="K39:K42"/>
+    <mergeCell ref="L39:L42"/>
+    <mergeCell ref="B43:B47"/>
+    <mergeCell ref="C43:C47"/>
+    <mergeCell ref="D43:D47"/>
+    <mergeCell ref="E43:E47"/>
+    <mergeCell ref="F43:F47"/>
+    <mergeCell ref="G43:G47"/>
+    <mergeCell ref="H43:H47"/>
+    <mergeCell ref="I43:I47"/>
+    <mergeCell ref="B39:B42"/>
+    <mergeCell ref="C39:C42"/>
+    <mergeCell ref="D39:D42"/>
+    <mergeCell ref="E39:E42"/>
+    <mergeCell ref="F39:F42"/>
+    <mergeCell ref="G39:G42"/>
+    <mergeCell ref="H39:H42"/>
+    <mergeCell ref="I39:I42"/>
+    <mergeCell ref="J39:J42"/>
+    <mergeCell ref="K32:K38"/>
+    <mergeCell ref="L32:L38"/>
+    <mergeCell ref="B32:B38"/>
+    <mergeCell ref="C32:C38"/>
+    <mergeCell ref="D32:D38"/>
+    <mergeCell ref="E32:E38"/>
+    <mergeCell ref="F32:F38"/>
+    <mergeCell ref="G32:G38"/>
+    <mergeCell ref="H32:H38"/>
+    <mergeCell ref="I32:I38"/>
+    <mergeCell ref="J32:J38"/>
+    <mergeCell ref="L11:L16"/>
+    <mergeCell ref="H24:H27"/>
+    <mergeCell ref="I24:I27"/>
+    <mergeCell ref="J24:J27"/>
+    <mergeCell ref="K24:K27"/>
+    <mergeCell ref="L24:L27"/>
+    <mergeCell ref="B28:B31"/>
+    <mergeCell ref="C28:C31"/>
+    <mergeCell ref="D28:D31"/>
+    <mergeCell ref="E28:E31"/>
+    <mergeCell ref="F28:F31"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="C24:C27"/>
+    <mergeCell ref="D24:D27"/>
+    <mergeCell ref="E24:E27"/>
+    <mergeCell ref="F24:F27"/>
+    <mergeCell ref="G24:G27"/>
+    <mergeCell ref="G28:G31"/>
+    <mergeCell ref="H28:H31"/>
+    <mergeCell ref="I28:I31"/>
+    <mergeCell ref="J28:J31"/>
+    <mergeCell ref="K28:K31"/>
+    <mergeCell ref="L28:L31"/>
+    <mergeCell ref="B17:B23"/>
     <mergeCell ref="C17:C23"/>
     <mergeCell ref="D17:D23"/>
     <mergeCell ref="E17:E23"/>
@@ -7497,254 +7743,32 @@
     <mergeCell ref="J11:J16"/>
     <mergeCell ref="K11:K16"/>
     <mergeCell ref="B7:B8"/>
-    <mergeCell ref="L11:L16"/>
-    <mergeCell ref="H24:H27"/>
-    <mergeCell ref="I24:I27"/>
-    <mergeCell ref="J24:J27"/>
-    <mergeCell ref="K24:K27"/>
-    <mergeCell ref="L24:L27"/>
-    <mergeCell ref="B28:B31"/>
-    <mergeCell ref="C28:C31"/>
-    <mergeCell ref="D28:D31"/>
-    <mergeCell ref="E28:E31"/>
-    <mergeCell ref="F28:F31"/>
-    <mergeCell ref="B24:B27"/>
-    <mergeCell ref="C24:C27"/>
-    <mergeCell ref="D24:D27"/>
-    <mergeCell ref="E24:E27"/>
-    <mergeCell ref="F24:F27"/>
-    <mergeCell ref="G24:G27"/>
-    <mergeCell ref="G28:G31"/>
-    <mergeCell ref="H28:H31"/>
-    <mergeCell ref="I28:I31"/>
-    <mergeCell ref="J28:J31"/>
-    <mergeCell ref="K28:K31"/>
-    <mergeCell ref="L28:L31"/>
-    <mergeCell ref="B17:B23"/>
-    <mergeCell ref="J39:J42"/>
-    <mergeCell ref="K32:K38"/>
-    <mergeCell ref="L32:L38"/>
-    <mergeCell ref="B32:B38"/>
-    <mergeCell ref="C32:C38"/>
-    <mergeCell ref="D32:D38"/>
-    <mergeCell ref="E32:E38"/>
-    <mergeCell ref="F32:F38"/>
-    <mergeCell ref="G32:G38"/>
-    <mergeCell ref="H32:H38"/>
-    <mergeCell ref="I32:I38"/>
-    <mergeCell ref="J32:J38"/>
-    <mergeCell ref="B48:B53"/>
-    <mergeCell ref="C48:C53"/>
-    <mergeCell ref="D48:D53"/>
-    <mergeCell ref="E48:E53"/>
-    <mergeCell ref="F48:F53"/>
-    <mergeCell ref="G48:G53"/>
-    <mergeCell ref="K39:K42"/>
-    <mergeCell ref="L39:L42"/>
-    <mergeCell ref="B43:B47"/>
-    <mergeCell ref="C43:C47"/>
-    <mergeCell ref="D43:D47"/>
-    <mergeCell ref="E43:E47"/>
-    <mergeCell ref="F43:F47"/>
-    <mergeCell ref="G43:G47"/>
-    <mergeCell ref="H43:H47"/>
-    <mergeCell ref="I43:I47"/>
-    <mergeCell ref="B39:B42"/>
-    <mergeCell ref="C39:C42"/>
-    <mergeCell ref="D39:D42"/>
-    <mergeCell ref="E39:E42"/>
-    <mergeCell ref="F39:F42"/>
-    <mergeCell ref="G39:G42"/>
-    <mergeCell ref="H39:H42"/>
-    <mergeCell ref="I39:I42"/>
-    <mergeCell ref="H48:H53"/>
-    <mergeCell ref="I48:I53"/>
-    <mergeCell ref="J48:J53"/>
-    <mergeCell ref="K48:K53"/>
-    <mergeCell ref="L48:L53"/>
-    <mergeCell ref="J43:J47"/>
-    <mergeCell ref="K43:K47"/>
-    <mergeCell ref="L43:L47"/>
-    <mergeCell ref="N43:N47"/>
-    <mergeCell ref="N48:N49"/>
-    <mergeCell ref="B59:B63"/>
-    <mergeCell ref="C59:C63"/>
-    <mergeCell ref="D59:D63"/>
-    <mergeCell ref="E59:E63"/>
-    <mergeCell ref="F59:F63"/>
-    <mergeCell ref="B54:B58"/>
-    <mergeCell ref="C54:C58"/>
-    <mergeCell ref="D54:D58"/>
-    <mergeCell ref="E54:E58"/>
-    <mergeCell ref="F54:F58"/>
-    <mergeCell ref="G59:G63"/>
-    <mergeCell ref="H59:H63"/>
-    <mergeCell ref="I59:I63"/>
-    <mergeCell ref="J59:J63"/>
-    <mergeCell ref="K59:K63"/>
-    <mergeCell ref="L59:L63"/>
-    <mergeCell ref="H54:H58"/>
-    <mergeCell ref="I54:I58"/>
-    <mergeCell ref="J54:J58"/>
-    <mergeCell ref="K54:K58"/>
-    <mergeCell ref="L54:L58"/>
-    <mergeCell ref="G54:G58"/>
-    <mergeCell ref="H67:H70"/>
-    <mergeCell ref="I67:I70"/>
-    <mergeCell ref="J67:J70"/>
-    <mergeCell ref="K67:K70"/>
-    <mergeCell ref="L67:L70"/>
-    <mergeCell ref="N67:N70"/>
-    <mergeCell ref="B67:B70"/>
-    <mergeCell ref="C67:C70"/>
-    <mergeCell ref="D67:D70"/>
-    <mergeCell ref="E67:E70"/>
-    <mergeCell ref="F67:F70"/>
-    <mergeCell ref="G67:G70"/>
-    <mergeCell ref="H71:H74"/>
-    <mergeCell ref="I71:I74"/>
-    <mergeCell ref="J71:J74"/>
-    <mergeCell ref="K71:K74"/>
-    <mergeCell ref="L71:L74"/>
-    <mergeCell ref="N71:N74"/>
-    <mergeCell ref="B71:B74"/>
-    <mergeCell ref="C71:C74"/>
-    <mergeCell ref="D71:D74"/>
-    <mergeCell ref="E71:E74"/>
-    <mergeCell ref="F71:F74"/>
-    <mergeCell ref="G71:G74"/>
-    <mergeCell ref="N75:N79"/>
-    <mergeCell ref="B80:B83"/>
-    <mergeCell ref="C80:C83"/>
-    <mergeCell ref="D80:D83"/>
-    <mergeCell ref="E80:E83"/>
-    <mergeCell ref="F80:F83"/>
-    <mergeCell ref="G80:G83"/>
-    <mergeCell ref="H80:H83"/>
-    <mergeCell ref="I80:I83"/>
-    <mergeCell ref="J80:J83"/>
-    <mergeCell ref="G75:G79"/>
-    <mergeCell ref="H75:H79"/>
-    <mergeCell ref="I75:I79"/>
-    <mergeCell ref="J75:J79"/>
-    <mergeCell ref="K75:K79"/>
-    <mergeCell ref="L75:L79"/>
-    <mergeCell ref="B75:B79"/>
-    <mergeCell ref="C75:C79"/>
-    <mergeCell ref="D75:D79"/>
-    <mergeCell ref="E75:E79"/>
-    <mergeCell ref="F75:F79"/>
-    <mergeCell ref="K80:K83"/>
-    <mergeCell ref="L80:L83"/>
-    <mergeCell ref="N80:N83"/>
-    <mergeCell ref="K84:K87"/>
-    <mergeCell ref="L84:L87"/>
-    <mergeCell ref="N84:N87"/>
-    <mergeCell ref="B88:B93"/>
-    <mergeCell ref="C88:C93"/>
-    <mergeCell ref="D88:D93"/>
-    <mergeCell ref="E88:E93"/>
-    <mergeCell ref="F88:F93"/>
-    <mergeCell ref="N88:N93"/>
-    <mergeCell ref="G88:G93"/>
-    <mergeCell ref="H88:H93"/>
-    <mergeCell ref="I88:I93"/>
-    <mergeCell ref="J88:J93"/>
-    <mergeCell ref="K88:K93"/>
-    <mergeCell ref="L88:L93"/>
-    <mergeCell ref="B84:B87"/>
-    <mergeCell ref="C84:C87"/>
-    <mergeCell ref="D84:D87"/>
-    <mergeCell ref="E84:E87"/>
-    <mergeCell ref="F84:F87"/>
-    <mergeCell ref="G84:G87"/>
-    <mergeCell ref="H84:H87"/>
-    <mergeCell ref="I84:I87"/>
-    <mergeCell ref="J84:J87"/>
-    <mergeCell ref="B94:B100"/>
-    <mergeCell ref="C94:C100"/>
-    <mergeCell ref="D94:D100"/>
-    <mergeCell ref="E94:E100"/>
-    <mergeCell ref="F94:F100"/>
-    <mergeCell ref="G94:G100"/>
-    <mergeCell ref="H94:H100"/>
-    <mergeCell ref="I94:I100"/>
-    <mergeCell ref="J94:J100"/>
-    <mergeCell ref="B106:B108"/>
-    <mergeCell ref="C106:C108"/>
-    <mergeCell ref="D106:D108"/>
-    <mergeCell ref="E106:E108"/>
-    <mergeCell ref="F106:F108"/>
-    <mergeCell ref="K94:K100"/>
-    <mergeCell ref="L94:L100"/>
-    <mergeCell ref="N94:N100"/>
-    <mergeCell ref="B101:B105"/>
-    <mergeCell ref="C101:C105"/>
-    <mergeCell ref="D101:D105"/>
-    <mergeCell ref="E101:E105"/>
-    <mergeCell ref="F101:F105"/>
-    <mergeCell ref="G101:G105"/>
-    <mergeCell ref="H101:H105"/>
-    <mergeCell ref="N106:N108"/>
-    <mergeCell ref="G106:G108"/>
-    <mergeCell ref="H106:H108"/>
-    <mergeCell ref="I106:I108"/>
-    <mergeCell ref="J106:J108"/>
-    <mergeCell ref="K106:K108"/>
-    <mergeCell ref="L106:L108"/>
-    <mergeCell ref="I101:I105"/>
-    <mergeCell ref="J101:J105"/>
-    <mergeCell ref="K101:K105"/>
-    <mergeCell ref="L101:L105"/>
-    <mergeCell ref="N101:N105"/>
-    <mergeCell ref="H110:H113"/>
-    <mergeCell ref="I110:I113"/>
-    <mergeCell ref="J110:J113"/>
-    <mergeCell ref="K110:K113"/>
-    <mergeCell ref="L110:L113"/>
-    <mergeCell ref="N110:N113"/>
-    <mergeCell ref="B110:B113"/>
-    <mergeCell ref="C110:C113"/>
-    <mergeCell ref="D110:D113"/>
-    <mergeCell ref="E110:E113"/>
-    <mergeCell ref="F110:F113"/>
-    <mergeCell ref="G110:G113"/>
-    <mergeCell ref="H114:H117"/>
-    <mergeCell ref="I114:I117"/>
-    <mergeCell ref="J114:J117"/>
-    <mergeCell ref="K114:K117"/>
-    <mergeCell ref="L114:L117"/>
-    <mergeCell ref="N114:N117"/>
-    <mergeCell ref="B114:B117"/>
-    <mergeCell ref="C114:C117"/>
-    <mergeCell ref="D114:D117"/>
-    <mergeCell ref="E114:E117"/>
-    <mergeCell ref="F114:F117"/>
-    <mergeCell ref="G114:G117"/>
-    <mergeCell ref="H118:H120"/>
-    <mergeCell ref="I118:I120"/>
-    <mergeCell ref="J118:J120"/>
-    <mergeCell ref="K118:K120"/>
-    <mergeCell ref="L118:L120"/>
-    <mergeCell ref="N118:N120"/>
-    <mergeCell ref="B118:B120"/>
-    <mergeCell ref="C118:C120"/>
-    <mergeCell ref="D118:D120"/>
-    <mergeCell ref="E118:E120"/>
-    <mergeCell ref="F118:F120"/>
-    <mergeCell ref="G118:G120"/>
-    <mergeCell ref="H122:H125"/>
-    <mergeCell ref="I122:I125"/>
-    <mergeCell ref="J122:J125"/>
-    <mergeCell ref="K122:K125"/>
-    <mergeCell ref="L122:L125"/>
-    <mergeCell ref="N122:N125"/>
-    <mergeCell ref="B122:B125"/>
-    <mergeCell ref="C122:C125"/>
-    <mergeCell ref="D122:D125"/>
-    <mergeCell ref="E122:E125"/>
-    <mergeCell ref="F122:F125"/>
-    <mergeCell ref="G122:G125"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="M3:N3"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="M5:M6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
CAN Adaptor placed & tracked - neesd poly pours adding Logos added Need to sort fob routing
</commit_message>
<xml_diff>
--- a/Karman Delta Arm/Rocket arming system.xlsx
+++ b/Karman Delta Arm/Rocket arming system.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adria\Documents\GitHub\AltiumGithub\Karman Delta Arm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83159B67-4154-458D-B4A4-41D4EA42FB8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DFB4E95-6CA4-4C5B-A7E9-3598E1CE5C26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="37965" yWindow="2010" windowWidth="21600" windowHeight="12645" tabRatio="745" activeTab="4" xr2:uid="{C397F53C-48EF-47A2-AFE9-4806826F5736}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="399">
   <si>
     <t>Failure Mode</t>
   </si>
@@ -1268,6 +1268,12 @@
   </si>
   <si>
     <t>Sort transceiver 3D body shape - currently on layer 1</t>
+  </si>
+  <si>
+    <t>Label Inputs &amp; Outputs</t>
+  </si>
+  <si>
+    <t>Check Poly Fills for unconnected copper</t>
   </si>
 </sst>
 </file>
@@ -3904,10 +3910,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90E11162-B732-4DE9-8322-FD8094AB6283}">
-  <dimension ref="A1:C49"/>
+  <dimension ref="A1:C51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -4196,6 +4202,9 @@
       <c r="A41" s="1" t="s">
         <v>388</v>
       </c>
+      <c r="B41" s="6" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="1" t="s">
@@ -4240,10 +4249,23 @@
       <c r="A48" s="1" t="s">
         <v>395</v>
       </c>
+      <c r="B48" s="6" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="49" spans="1:1" ht="30">
       <c r="A49" s="1" t="s">
         <v>396</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" s="1" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" s="1" t="s">
+        <v>398</v>
       </c>
     </row>
   </sheetData>

</xml_diff>